<commit_message>
updated scalers for 8-ch board
add per-channel scalers for all 8 channels. Now 20 scalers per scaler type (1Hz, 1Hz-gated, 100Hz)
</commit_message>
<xml_diff>
--- a/doc/flower8-register-map.xlsx
+++ b/doc/flower8-register-map.xlsx
@@ -452,9 +452,6 @@
     <t>note channel 5 hard-coded masked from trigger (dead vpol channel)</t>
   </si>
   <si>
-    <t>FLOWER board</t>
-  </si>
-  <si>
     <t xml:space="preserve">REMOTE FIRMWARE PROGRAMMING </t>
   </si>
   <si>
@@ -618,6 +615,9 @@
   </si>
   <si>
     <t>register address moved in FLOWER8</t>
+  </si>
+  <si>
+    <t>FLOWER board w/8channel firmware</t>
   </si>
 </sst>
 </file>
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D85" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,7 +1225,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>139</v>
+        <v>194</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="57">
-        <v>44212</v>
+        <v>45170</v>
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="1"/>
@@ -1425,7 +1425,7 @@
         <v>40</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1470,7 +1470,7 @@
         <v>x0A</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>47</v>
@@ -1492,7 +1492,7 @@
         <v>x0B</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>47</v>
@@ -1512,7 +1512,7 @@
         <v>x0C</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>47</v>
@@ -1532,7 +1532,7 @@
         <v>x0D</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>47</v>
@@ -1552,10 +1552,10 @@
         <v>x0E</v>
       </c>
       <c r="C21" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D21" s="18" t="s">
         <v>175</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>176</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>6</v>
@@ -1835,7 +1835,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D41" s="43"/>
       <c r="E41" s="43"/>
@@ -1971,7 +1971,7 @@
         <v>43</v>
       </c>
       <c r="D48" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E48" t="s">
         <v>6</v>
@@ -1993,7 +1993,7 @@
         <v>29</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E49" t="s">
         <v>6</v>
@@ -2176,13 +2176,13 @@
         <v>21</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2198,13 +2198,13 @@
         <v>22</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2217,10 +2217,10 @@
         <v>x3A</v>
       </c>
       <c r="C65" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="E65" s="34" t="s">
         <v>6</v>
@@ -2236,10 +2236,10 @@
         <v>x3B</v>
       </c>
       <c r="C66" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="E66" s="34" t="s">
         <v>6</v>
@@ -2255,10 +2255,10 @@
         <v>x3C</v>
       </c>
       <c r="C67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E67" s="34" t="s">
         <v>6</v>
@@ -2274,10 +2274,10 @@
         <v>x3D</v>
       </c>
       <c r="C68" t="s">
+        <v>163</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="E68" s="45" t="s">
         <v>6</v>
@@ -2358,13 +2358,13 @@
         <v>x42</v>
       </c>
       <c r="C73" t="s">
+        <v>150</v>
+      </c>
+      <c r="D73" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D73" s="5" t="s">
-        <v>152</v>
-      </c>
       <c r="F73" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2388,16 +2388,16 @@
         <v>x44</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F75" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2536,13 +2536,13 @@
         <v>35</v>
       </c>
       <c r="D83" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E83" t="s">
+        <v>178</v>
+      </c>
+      <c r="F83" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="E83" t="s">
-        <v>179</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
         <v>78</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E84" t="s">
         <v>7</v>
@@ -2742,16 +2742,16 @@
         <v>x56</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="94" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2764,10 +2764,10 @@
         <v>x57</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>7</v>
@@ -2784,10 +2784,10 @@
         <v>x58</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>7</v>
@@ -2804,10 +2804,10 @@
         <v>x59</v>
       </c>
       <c r="C96" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D96" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>159</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>7</v>
@@ -2824,10 +2824,10 @@
         <v>x5A</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>7</v>
@@ -2844,10 +2844,10 @@
         <v>x5B</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>7</v>
@@ -2864,10 +2864,10 @@
         <v>x5C</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>7</v>
@@ -2884,10 +2884,10 @@
         <v>x5D</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>7</v>
@@ -2904,10 +2904,10 @@
         <v>x5E</v>
       </c>
       <c r="C101" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D101" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="E101" s="55" t="s">
         <v>11</v>
@@ -2923,13 +2923,13 @@
         <v>x5F</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F102" s="7"/>
     </row>
@@ -2943,10 +2943,10 @@
         <v>x60</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>11</v>
@@ -2963,10 +2963,10 @@
         <v>x61</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>7</v>
@@ -3060,7 +3060,7 @@
         <v>116</v>
       </c>
       <c r="F110" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="111" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3076,7 +3076,7 @@
         <v>113</v>
       </c>
       <c r="F111" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="112" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3092,7 +3092,7 @@
         <v>114</v>
       </c>
       <c r="F112" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="113" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
         <v>117</v>
       </c>
       <c r="F113" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="114" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3124,7 +3124,7 @@
         <v>118</v>
       </c>
       <c r="F114" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3187,7 +3187,7 @@
         <v>99</v>
       </c>
       <c r="F117" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="118" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3206,7 +3206,7 @@
         <v>97</v>
       </c>
       <c r="F118" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="119" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3225,7 +3225,7 @@
         <v>98</v>
       </c>
       <c r="F119" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="120" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3244,7 +3244,7 @@
         <v>98</v>
       </c>
       <c r="F120" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="121" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3263,7 +3263,7 @@
         <v>107</v>
       </c>
       <c r="F121" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="122" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3282,7 +3282,7 @@
         <v>98</v>
       </c>
       <c r="F122" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="123" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3301,7 +3301,7 @@
         <v>98</v>
       </c>
       <c r="F123" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="124" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3320,7 +3320,7 @@
         <v>109</v>
       </c>
       <c r="F124" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="125" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3339,7 +3339,7 @@
         <v>98</v>
       </c>
       <c r="F125" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="126" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3358,7 +3358,7 @@
         <v>98</v>
       </c>
       <c r="F126" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="127" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3374,7 +3374,7 @@
         <v>119</v>
       </c>
       <c r="F127" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="128" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3393,7 +3393,7 @@
         <v>115</v>
       </c>
       <c r="F128" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3416,10 +3416,10 @@
         <v>x7B</v>
       </c>
       <c r="C130" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="F130" s="40" t="s">
         <v>142</v>
-      </c>
-      <c r="F130" s="40" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="131" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -3432,10 +3432,10 @@
         <v>x7C</v>
       </c>
       <c r="C131" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F131" s="40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -3488,7 +3488,7 @@
         <v>7</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2-board syncing firmware added
compiles, not tested
</commit_message>
<xml_diff>
--- a/doc/flower8-register-map.xlsx
+++ b/doc/flower8-register-map.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="197">
   <si>
     <t>Register Map</t>
   </si>
@@ -618,13 +618,19 @@
   </si>
   <si>
     <t>FLOWER board w/8channel firmware</t>
+  </si>
+  <si>
+    <t>sync reg</t>
+  </si>
+  <si>
+    <t>LSB=1, then board is master. If a 2 is written then board is slave. If syncing a command, slave board needs to be assigned *first*, which makes board look at ext_trig_in for a sync. Then assigning master board register makes ext_trig_out the sync signal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -708,6 +714,14 @@
       <strike/>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -813,7 +827,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -920,11 +934,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1208,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,38 +1242,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="57">
+      <c r="A4" s="58">
         <v>45170</v>
       </c>
-      <c r="B4" s="58"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>37</v>
@@ -2737,7 +2755,7 @@
         <f t="shared" si="3"/>
         <v>86</v>
       </c>
-      <c r="B93" s="59" t="str">
+      <c r="B93" s="56" t="str">
         <f t="shared" si="2"/>
         <v>x56</v>
       </c>
@@ -2759,7 +2777,7 @@
         <f t="shared" si="3"/>
         <v>87</v>
       </c>
-      <c r="B94" s="59" t="str">
+      <c r="B94" s="56" t="str">
         <f t="shared" si="2"/>
         <v>x57</v>
       </c>
@@ -2779,7 +2797,7 @@
         <f t="shared" si="3"/>
         <v>88</v>
       </c>
-      <c r="B95" s="59" t="str">
+      <c r="B95" s="56" t="str">
         <f t="shared" si="2"/>
         <v>x58</v>
       </c>
@@ -2799,7 +2817,7 @@
         <f t="shared" si="3"/>
         <v>89</v>
       </c>
-      <c r="B96" s="59" t="str">
+      <c r="B96" s="56" t="str">
         <f t="shared" si="2"/>
         <v>x59</v>
       </c>
@@ -2819,7 +2837,7 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="B97" s="59" t="str">
+      <c r="B97" s="56" t="str">
         <f t="shared" si="2"/>
         <v>x5A</v>
       </c>
@@ -2839,7 +2857,7 @@
         <f t="shared" si="3"/>
         <v>91</v>
       </c>
-      <c r="B98" s="59" t="str">
+      <c r="B98" s="56" t="str">
         <f t="shared" si="2"/>
         <v>x5B</v>
       </c>
@@ -2859,7 +2877,7 @@
         <f t="shared" si="3"/>
         <v>92</v>
       </c>
-      <c r="B99" s="59" t="str">
+      <c r="B99" s="56" t="str">
         <f t="shared" si="2"/>
         <v>x5C</v>
       </c>
@@ -2879,7 +2897,7 @@
         <f t="shared" si="3"/>
         <v>93</v>
       </c>
-      <c r="B100" s="59" t="str">
+      <c r="B100" s="56" t="str">
         <f t="shared" si="2"/>
         <v>x5D</v>
       </c>
@@ -2918,7 +2936,7 @@
         <f t="shared" si="3"/>
         <v>95</v>
       </c>
-      <c r="B102" s="59" t="str">
+      <c r="B102" s="56" t="str">
         <f t="shared" si="2"/>
         <v>x5F</v>
       </c>
@@ -2938,7 +2956,7 @@
         <f t="shared" si="3"/>
         <v>96</v>
       </c>
-      <c r="B103" s="59" t="str">
+      <c r="B103" s="56" t="str">
         <f t="shared" si="2"/>
         <v>x60</v>
       </c>
@@ -2958,7 +2976,7 @@
         <f t="shared" si="3"/>
         <v>97</v>
       </c>
-      <c r="B104" s="59" t="str">
+      <c r="B104" s="56" t="str">
         <f t="shared" si="2"/>
         <v>x61</v>
       </c>
@@ -2986,7 +3004,7 @@
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A106">
         <f t="shared" si="3"/>
         <v>99</v>
@@ -2995,9 +3013,15 @@
         <f t="shared" si="2"/>
         <v>x63</v>
       </c>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
+      <c r="C106" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="D106" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="E106" s="60" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
@@ -3008,9 +3032,9 @@
         <f t="shared" si="2"/>
         <v>x64</v>
       </c>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
+      <c r="C107" s="60"/>
+      <c r="D107" s="61"/>
+      <c r="E107" s="60"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">

</xml_diff>

<commit_message>
udpate doc w/ scaler map
</commit_message>
<xml_diff>
--- a/doc/flower8-register-map.xlsx
+++ b/doc/flower8-register-map.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="600" windowWidth="23235" windowHeight="14700"/>
+    <workbookView xWindow="1455" yWindow="600" windowWidth="23235" windowHeight="14700" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="registers" sheetId="1" r:id="rId1"/>
+    <sheet name="scalers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="229">
   <si>
     <t>Register Map</t>
   </si>
@@ -624,6 +625,102 @@
   </si>
   <si>
     <t>toggle FPGA-generated fast pulse w/ LSB, toggle RF switch with LSB+1, bit8 is freq select (0=fastest, 1=8x slower), bit16 is the pps sync option</t>
+  </si>
+  <si>
+    <t>software trig_type=1 ; external trig_type=2; coinc trig_type=3; phase trig_type=4, internal pps_trig_type=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCALER # </t>
+  </si>
+  <si>
+    <t>update rate</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>1Hz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaler adr </t>
+  </si>
+  <si>
+    <t>coincidence trig</t>
+  </si>
+  <si>
+    <t>ch0 singles</t>
+  </si>
+  <si>
+    <t>ch1 singles</t>
+  </si>
+  <si>
+    <t>ch3 singles</t>
+  </si>
+  <si>
+    <t>ch2 singles</t>
+  </si>
+  <si>
+    <t>ch4 singles</t>
+  </si>
+  <si>
+    <t>ch5 singles</t>
+  </si>
+  <si>
+    <t>ch6 singles</t>
+  </si>
+  <si>
+    <t>ch7 singles</t>
+  </si>
+  <si>
+    <t>coincidence servo</t>
+  </si>
+  <si>
+    <t>ch0 servo</t>
+  </si>
+  <si>
+    <t>ch1 servo</t>
+  </si>
+  <si>
+    <t>ch2 servo</t>
+  </si>
+  <si>
+    <t>ch3 servo</t>
+  </si>
+  <si>
+    <t>ch4 servo</t>
+  </si>
+  <si>
+    <t>ch5 servo</t>
+  </si>
+  <si>
+    <t>ch6 servo</t>
+  </si>
+  <si>
+    <t>ch7 servo</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>gated 1Hz</t>
+  </si>
+  <si>
+    <t>100Hz</t>
+  </si>
+  <si>
+    <t>1Hz scaler update counter</t>
+  </si>
+  <si>
+    <t>all 12 bits -- 2 scalers per scaler adr</t>
+  </si>
+  <si>
+    <t>latched pps counter (lower 24 bits)</t>
+  </si>
+  <si>
+    <t>latched pps counter (upper 24 bits)</t>
+  </si>
+  <si>
+    <t>will change to 0.1Hz</t>
   </si>
 </sst>
 </file>
@@ -835,7 +932,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -950,6 +1047,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1235,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,38 +1349,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>193</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="61">
+      <c r="A4" s="62">
         <v>45170</v>
       </c>
-      <c r="B4" s="62"/>
+      <c r="B4" s="63"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>37</v>
@@ -1569,7 +1667,7 @@
       </c>
       <c r="F20" s="19"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1587,7 +1685,9 @@
       <c r="E21" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="19" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
@@ -3535,4 +3635,1009 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="60" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="60">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="60">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="60">
+        <f t="shared" ref="A4:A63" si="0">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="60">
+        <v>1</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="60">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="60">
+        <v>1</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="60">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="60">
+        <v>2</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="60">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="60">
+        <v>2</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="60">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="60">
+        <v>3</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="60">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="60">
+        <v>3</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="60">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="60">
+        <v>4</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="60">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="60">
+        <v>4</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>212</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="60">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="60">
+        <v>5</v>
+      </c>
+      <c r="C12" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="60">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="60">
+        <v>5</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>214</v>
+      </c>
+      <c r="D13" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="60">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="60">
+        <v>6</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>215</v>
+      </c>
+      <c r="D14" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="60">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="60">
+        <v>6</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>216</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="60">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="60">
+        <v>7</v>
+      </c>
+      <c r="C16" s="60" t="s">
+        <v>217</v>
+      </c>
+      <c r="D16" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="60">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="60">
+        <v>7</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>218</v>
+      </c>
+      <c r="D17" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="60">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="60">
+        <v>8</v>
+      </c>
+      <c r="C18" s="60" t="s">
+        <v>219</v>
+      </c>
+      <c r="D18" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="60">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="60">
+        <v>8</v>
+      </c>
+      <c r="C19" s="60" t="s">
+        <v>220</v>
+      </c>
+      <c r="D19" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="60">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="60">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>221</v>
+      </c>
+      <c r="D20" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="60">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="60">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>221</v>
+      </c>
+      <c r="D21" s="60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="60">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="60">
+        <v>10</v>
+      </c>
+      <c r="C22" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="D22" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="60">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="60">
+        <v>10</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>204</v>
+      </c>
+      <c r="D23" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="60">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="60">
+        <v>11</v>
+      </c>
+      <c r="C24" s="60" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="60">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="60">
+        <v>11</v>
+      </c>
+      <c r="C25" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="D25" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="60">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="60">
+        <v>12</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>206</v>
+      </c>
+      <c r="D26" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="60">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="60">
+        <v>12</v>
+      </c>
+      <c r="C27" s="60" t="s">
+        <v>208</v>
+      </c>
+      <c r="D27" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="60">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="60">
+        <v>13</v>
+      </c>
+      <c r="C28" s="60" t="s">
+        <v>209</v>
+      </c>
+      <c r="D28" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="60">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="60">
+        <v>13</v>
+      </c>
+      <c r="C29" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="D29" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="60">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="60">
+        <v>14</v>
+      </c>
+      <c r="C30" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="D30" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="60">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="60">
+        <v>14</v>
+      </c>
+      <c r="C31" s="60" t="s">
+        <v>212</v>
+      </c>
+      <c r="D31" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="60">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="60">
+        <v>15</v>
+      </c>
+      <c r="C32" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="D32" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="60">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="60">
+        <v>15</v>
+      </c>
+      <c r="C33" s="60" t="s">
+        <v>214</v>
+      </c>
+      <c r="D33" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="60">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="60">
+        <v>16</v>
+      </c>
+      <c r="C34" s="60" t="s">
+        <v>215</v>
+      </c>
+      <c r="D34" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="60">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="60">
+        <v>16</v>
+      </c>
+      <c r="C35" s="60" t="s">
+        <v>216</v>
+      </c>
+      <c r="D35" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="60">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="60">
+        <v>17</v>
+      </c>
+      <c r="C36" s="60" t="s">
+        <v>217</v>
+      </c>
+      <c r="D36" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="60">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="60">
+        <v>17</v>
+      </c>
+      <c r="C37" s="60" t="s">
+        <v>218</v>
+      </c>
+      <c r="D37" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="60">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B38" s="60">
+        <v>18</v>
+      </c>
+      <c r="C38" s="60" t="s">
+        <v>219</v>
+      </c>
+      <c r="D38" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="60">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B39" s="60">
+        <v>18</v>
+      </c>
+      <c r="C39" s="60" t="s">
+        <v>220</v>
+      </c>
+      <c r="D39" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="60">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B40" s="60">
+        <v>19</v>
+      </c>
+      <c r="C40" s="60" t="s">
+        <v>221</v>
+      </c>
+      <c r="D40" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="60">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B41" s="60">
+        <v>19</v>
+      </c>
+      <c r="C41" s="60" t="s">
+        <v>221</v>
+      </c>
+      <c r="D41" s="60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="60">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B42" s="60">
+        <v>20</v>
+      </c>
+      <c r="C42" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="D42" t="s">
+        <v>223</v>
+      </c>
+      <c r="E42" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="60">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B43" s="60">
+        <v>20</v>
+      </c>
+      <c r="C43" s="60" t="s">
+        <v>204</v>
+      </c>
+      <c r="D43" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="60">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B44" s="60">
+        <v>21</v>
+      </c>
+      <c r="C44" s="60" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="60">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B45" s="60">
+        <v>21</v>
+      </c>
+      <c r="C45" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="60">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B46" s="60">
+        <v>22</v>
+      </c>
+      <c r="C46" s="60" t="s">
+        <v>206</v>
+      </c>
+      <c r="D46" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="60">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B47" s="60">
+        <v>22</v>
+      </c>
+      <c r="C47" s="60" t="s">
+        <v>208</v>
+      </c>
+      <c r="D47" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="60">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B48" s="60">
+        <v>23</v>
+      </c>
+      <c r="C48" s="60" t="s">
+        <v>209</v>
+      </c>
+      <c r="D48" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="60">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B49" s="60">
+        <v>23</v>
+      </c>
+      <c r="C49" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="D49" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="60">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B50" s="60">
+        <v>24</v>
+      </c>
+      <c r="C50" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="D50" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="60">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B51" s="60">
+        <v>24</v>
+      </c>
+      <c r="C51" s="60" t="s">
+        <v>212</v>
+      </c>
+      <c r="D51" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="60">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B52" s="60">
+        <v>25</v>
+      </c>
+      <c r="C52" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="D52" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="60">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B53" s="60">
+        <v>25</v>
+      </c>
+      <c r="C53" s="60" t="s">
+        <v>214</v>
+      </c>
+      <c r="D53" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="60">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B54" s="60">
+        <v>26</v>
+      </c>
+      <c r="C54" s="60" t="s">
+        <v>215</v>
+      </c>
+      <c r="D54" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="60">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B55" s="60">
+        <v>26</v>
+      </c>
+      <c r="C55" s="60" t="s">
+        <v>216</v>
+      </c>
+      <c r="D55" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="60">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B56" s="60">
+        <v>27</v>
+      </c>
+      <c r="C56" s="60" t="s">
+        <v>217</v>
+      </c>
+      <c r="D56" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="60">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B57" s="60">
+        <v>27</v>
+      </c>
+      <c r="C57" s="60" t="s">
+        <v>218</v>
+      </c>
+      <c r="D57" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="60">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B58" s="60">
+        <v>28</v>
+      </c>
+      <c r="C58" s="60" t="s">
+        <v>219</v>
+      </c>
+      <c r="D58" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="60">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B59" s="60">
+        <v>28</v>
+      </c>
+      <c r="C59" s="60" t="s">
+        <v>220</v>
+      </c>
+      <c r="D59" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="60">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B60" s="60">
+        <v>29</v>
+      </c>
+      <c r="C60" s="60" t="s">
+        <v>221</v>
+      </c>
+      <c r="D60" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="60">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B61" s="60">
+        <v>29</v>
+      </c>
+      <c r="C61" s="60" t="s">
+        <v>221</v>
+      </c>
+      <c r="D61" s="60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="60">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B62" s="60">
+        <v>30</v>
+      </c>
+      <c r="C62" s="60" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="60">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B63" s="60">
+        <v>30</v>
+      </c>
+      <c r="C63" s="60" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" s="60">
+        <v>31</v>
+      </c>
+      <c r="C64" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" s="60">
+        <v>31</v>
+      </c>
+      <c r="C65" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="60">
+        <v>32</v>
+      </c>
+      <c r="C66" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="60">
+        <v>33</v>
+      </c>
+      <c r="C67" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update to 20MHz FPGA global signal clocking,
also add 100mHz scalers
</commit_message>
<xml_diff>
--- a/doc/flower8-register-map.xlsx
+++ b/doc/flower8-register-map.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="233">
   <si>
     <t>Register Map</t>
   </si>
@@ -721,6 +721,18 @@
   </si>
   <si>
     <t>will change to 0.1Hz</t>
+  </si>
+  <si>
+    <t>sys trig out not used in terradaq/beacon/ dual flower8!!!</t>
+  </si>
+  <si>
+    <t>unused</t>
+  </si>
+  <si>
+    <t>set top scaler update rate to 100Hz or 100mHz</t>
+  </si>
+  <si>
+    <t>lsb=1 is 100Hz, lsb=0 is 100mHz [default]</t>
   </si>
 </sst>
 </file>
@@ -1333,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D5" sqref="D4:D5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,7 +2208,15 @@
         <f t="shared" si="0"/>
         <v>x2F</v>
       </c>
-      <c r="D54" s="5"/>
+      <c r="C54" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -2615,7 +2635,7 @@
       </c>
       <c r="E80" s="4"/>
     </row>
-    <row r="81" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <f t="shared" si="3"/>
         <v>74</v>
@@ -2628,7 +2648,7 @@
       <c r="D81" s="12"/>
       <c r="F81" s="10"/>
     </row>
-    <row r="82" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <f t="shared" si="3"/>
         <v>75</v>
@@ -2650,7 +2670,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="3"/>
         <v>76</v>
@@ -2672,7 +2692,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="3"/>
         <v>77</v>
@@ -2694,7 +2714,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="3"/>
         <v>78</v>
@@ -2716,7 +2736,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="3"/>
         <v>79</v>
@@ -2729,7 +2749,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="3"/>
         <v>80</v>
@@ -2750,8 +2770,11 @@
       <c r="F87" s="47" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="3"/>
         <v>81</v>
@@ -2772,8 +2795,11 @@
       <c r="F88" s="47" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="3"/>
         <v>82</v>
@@ -2794,8 +2820,11 @@
       <c r="F89" s="47" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G89" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="3"/>
         <v>83</v>
@@ -2816,8 +2845,11 @@
       <c r="F90" s="47" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G90" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="3"/>
         <v>84</v>
@@ -2838,8 +2870,11 @@
       <c r="F91" s="47" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G91" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="3"/>
         <v>85</v>
@@ -2859,7 +2894,7 @@
       </c>
       <c r="F92" s="47"/>
     </row>
-    <row r="93" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <f t="shared" si="3"/>
         <v>86</v>
@@ -2881,7 +2916,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <f t="shared" si="3"/>
         <v>87</v>
@@ -2901,7 +2936,7 @@
       </c>
       <c r="F94" s="7"/>
     </row>
-    <row r="95" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <f t="shared" si="3"/>
         <v>88</v>
@@ -2921,7 +2956,7 @@
       </c>
       <c r="F95" s="7"/>
     </row>
-    <row r="96" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <f t="shared" si="3"/>
         <v>89</v>
@@ -3078,7 +3113,9 @@
       <c r="E103" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F103" s="7"/>
+      <c r="F103" s="7" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="104" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="2">

</xml_diff>

<commit_message>
lots of (good) updates
</commit_message>
<xml_diff>
--- a/doc/flower8-register-map.xlsx
+++ b/doc/flower8-register-map.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="238">
   <si>
     <t>Register Map</t>
   </si>
@@ -733,6 +733,21 @@
   </si>
   <si>
     <t>lsb=1 is 100Hz, lsb=0 is 100mHz [default]</t>
+  </si>
+  <si>
+    <t>event metadata-&gt;trig</t>
+  </si>
+  <si>
+    <t>read_only - event meta data -- low 8 bits latched trigger channels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COINC TRIGGER-&gt; mask </t>
+  </si>
+  <si>
+    <t>lowest-byte is channel mask</t>
+  </si>
+  <si>
+    <t>x0000FF</t>
   </si>
 </sst>
 </file>
@@ -1345,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,6 +1725,12 @@
         <f t="shared" si="0"/>
         <v>x0F</v>
       </c>
+      <c r="C22" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>234</v>
+      </c>
       <c r="F22" s="19"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3146,9 +3167,15 @@
         <f t="shared" si="2"/>
         <v>x62</v>
       </c>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11"/>
+      <c r="C105" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A106">
@@ -3679,7 +3706,7 @@
   <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
now using more regs. 20 beams compiles. soft 26 beam limit in beam mask reg
</commit_message>
<xml_diff>
--- a/doc/flower8-register-map.xlsx
+++ b/doc/flower8-register-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryank\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9811BC1F-3E36-4C22-A80E-F98C90D88214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F721A7E5-9582-468C-AD2F-A37583CE8935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14505" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registers" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="241">
   <si>
     <t>Register Map</t>
   </si>
@@ -697,40 +697,58 @@
     <t>replacing with p-hased trigger</t>
   </si>
   <si>
-    <t>LSB-&gt; pps trig enable, middle byte LSB-&gt; phased trig enable, high byte LSB-&gt;ext trig enable</t>
-  </si>
-  <si>
     <t>beam 0 thresholds</t>
   </si>
   <si>
     <t>beam 1 thresholds</t>
   </si>
   <si>
-    <t>beam 2 thresholds</t>
-  </si>
-  <si>
-    <t>beam 3 thresholds</t>
-  </si>
-  <si>
-    <t>beam 4 thresholds</t>
-  </si>
-  <si>
-    <t>beam 5 thresholds</t>
-  </si>
-  <si>
-    <t>beam 6 thresholds</t>
-  </si>
-  <si>
-    <t>beam 7 thresholds</t>
-  </si>
-  <si>
-    <t>beam 8 thresholds</t>
-  </si>
-  <si>
-    <t>beam 9 thresholds</t>
-  </si>
-  <si>
     <t>RK 2/9/2024</t>
+  </si>
+  <si>
+    <t>Beam 0 Thresholds</t>
+  </si>
+  <si>
+    <t>Beam Threshold Block</t>
+  </si>
+  <si>
+    <t>0xffffff</t>
+  </si>
+  <si>
+    <t>COINC TRIGGER-&gt; threshold ch0</t>
+  </si>
+  <si>
+    <t>lowest byte : nominal trigger thresh ; middle byte : servo trigger threshold</t>
+  </si>
+  <si>
+    <t>register address moved in FLOWER8</t>
+  </si>
+  <si>
+    <t>COINC TRIGGER-&gt; threshold ch1</t>
+  </si>
+  <si>
+    <t>COINC TRIGGER-&gt; threshold ch2</t>
+  </si>
+  <si>
+    <t>COINC TRIGGER-&gt; threshold ch3</t>
+  </si>
+  <si>
+    <t>COINC TRIGGER-&gt; threshold ch4</t>
+  </si>
+  <si>
+    <t>COINC TRIGGER-&gt; threshold ch5</t>
+  </si>
+  <si>
+    <t>COINC TRIGGER-&gt; threshold ch6</t>
+  </si>
+  <si>
+    <t>COINC TRIGGER-&gt; threshold ch7</t>
+  </si>
+  <si>
+    <t>LSB-&gt; pps trig enable, middle byte LSB+1-&gt; phased trig enable,,middle byte LSB-&gt; coinc trig enable high byte LSB-&gt;ext trig enable</t>
+  </si>
+  <si>
+    <t>MS 12 bits = Servo Thresholds, LS 12 bits Trigger Thresholds</t>
   </si>
 </sst>
 </file>
@@ -942,7 +960,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1039,6 +1057,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1319,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G134"/>
+  <dimension ref="A1:G262"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="D132" workbookViewId="0">
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1391,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="45" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B4" s="44"/>
       <c r="C4" s="1"/>
@@ -2348,7 +2373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -2361,7 +2386,7 @@
         <v>150</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="E68" t="s">
         <v>6</v>
@@ -2796,7 +2821,7 @@
         <v>x54</v>
       </c>
       <c r="C91" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D91" s="32"/>
       <c r="E91" s="32" t="s">
@@ -2815,7 +2840,7 @@
         <v>x55</v>
       </c>
       <c r="C92" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D92" s="33"/>
       <c r="E92" s="32" t="s">
@@ -2832,14 +2857,18 @@
         <f t="shared" si="2"/>
         <v>x56</v>
       </c>
-      <c r="C93" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="D93" s="5"/>
+      <c r="C93" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>230</v>
+      </c>
       <c r="E93" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F93" s="5"/>
+      <c r="F93" s="5" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="94" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
@@ -2850,10 +2879,12 @@
         <f t="shared" si="2"/>
         <v>x57</v>
       </c>
-      <c r="C94" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="D94" s="5"/>
+      <c r="C94" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>230</v>
+      </c>
       <c r="E94" s="2" t="s">
         <v>7</v>
       </c>
@@ -2868,10 +2899,12 @@
         <f t="shared" si="2"/>
         <v>x58</v>
       </c>
-      <c r="C95" s="32" t="s">
-        <v>228</v>
-      </c>
-      <c r="D95" s="5"/>
+      <c r="C95" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>230</v>
+      </c>
       <c r="E95" s="2" t="s">
         <v>7</v>
       </c>
@@ -2886,10 +2919,12 @@
         <f t="shared" si="2"/>
         <v>x59</v>
       </c>
-      <c r="C96" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="D96" s="5"/>
+      <c r="C96" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>230</v>
+      </c>
       <c r="E96" s="2" t="s">
         <v>7</v>
       </c>
@@ -2904,10 +2939,12 @@
         <f t="shared" si="2"/>
         <v>x5A</v>
       </c>
-      <c r="C97" s="32" t="s">
+      <c r="C97" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D97" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="D97" s="5"/>
       <c r="E97" s="2" t="s">
         <v>7</v>
       </c>
@@ -2922,10 +2959,12 @@
         <f t="shared" si="2"/>
         <v>x5B</v>
       </c>
-      <c r="C98" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="D98" s="5"/>
+      <c r="C98" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>230</v>
+      </c>
       <c r="E98" s="2" t="s">
         <v>7</v>
       </c>
@@ -2940,10 +2979,12 @@
         <f t="shared" si="2"/>
         <v>x5C</v>
       </c>
-      <c r="C99" s="32" t="s">
-        <v>232</v>
-      </c>
-      <c r="D99" s="5"/>
+      <c r="C99" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>230</v>
+      </c>
       <c r="E99" s="2" t="s">
         <v>7</v>
       </c>
@@ -2958,10 +2999,12 @@
         <f t="shared" si="2"/>
         <v>x5D</v>
       </c>
-      <c r="C100" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="D100" s="5"/>
+      <c r="C100" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>230</v>
+      </c>
       <c r="E100" s="2" t="s">
         <v>7</v>
       </c>
@@ -3574,6 +3617,1175 @@
       </c>
       <c r="F134" s="3" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>128</v>
+      </c>
+      <c r="B135" t="str">
+        <f>"x" &amp; DEC2HEX(A135,2)</f>
+        <v>x80</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="10">
+        <v>129</v>
+      </c>
+      <c r="B136" s="10" t="str">
+        <f>"x" &amp; DEC2HEX(A136,2)</f>
+        <v>x81</v>
+      </c>
+      <c r="C136" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D136" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="E136" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="F136" s="46"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>130</v>
+      </c>
+      <c r="B137" t="str">
+        <f t="shared" ref="B137:B200" si="4">"x" &amp; DEC2HEX(A137,2)</f>
+        <v>x82</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>131</v>
+      </c>
+      <c r="B138" t="str">
+        <f t="shared" si="4"/>
+        <v>x83</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>132</v>
+      </c>
+      <c r="B139" t="str">
+        <f t="shared" si="4"/>
+        <v>x84</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>133</v>
+      </c>
+      <c r="B140" t="str">
+        <f t="shared" si="4"/>
+        <v>x85</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>134</v>
+      </c>
+      <c r="B141" t="str">
+        <f t="shared" si="4"/>
+        <v>x86</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>135</v>
+      </c>
+      <c r="B142" t="str">
+        <f t="shared" si="4"/>
+        <v>x87</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>136</v>
+      </c>
+      <c r="B143" t="str">
+        <f t="shared" si="4"/>
+        <v>x88</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>137</v>
+      </c>
+      <c r="B144" t="str">
+        <f t="shared" si="4"/>
+        <v>x89</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>138</v>
+      </c>
+      <c r="B145" t="str">
+        <f t="shared" si="4"/>
+        <v>x8A</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>139</v>
+      </c>
+      <c r="B146" t="str">
+        <f t="shared" si="4"/>
+        <v>x8B</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>140</v>
+      </c>
+      <c r="B147" t="str">
+        <f t="shared" si="4"/>
+        <v>x8C</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>141</v>
+      </c>
+      <c r="B148" t="str">
+        <f t="shared" si="4"/>
+        <v>x8D</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>142</v>
+      </c>
+      <c r="B149" t="str">
+        <f t="shared" si="4"/>
+        <v>x8E</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>143</v>
+      </c>
+      <c r="B150" t="str">
+        <f t="shared" si="4"/>
+        <v>x8F</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>144</v>
+      </c>
+      <c r="B151" t="str">
+        <f t="shared" si="4"/>
+        <v>x90</v>
+      </c>
+      <c r="C151" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>145</v>
+      </c>
+      <c r="B152" t="str">
+        <f t="shared" si="4"/>
+        <v>x91</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>146</v>
+      </c>
+      <c r="B153" t="str">
+        <f t="shared" si="4"/>
+        <v>x92</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>147</v>
+      </c>
+      <c r="B154" t="str">
+        <f t="shared" si="4"/>
+        <v>x93</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>148</v>
+      </c>
+      <c r="B155" t="str">
+        <f t="shared" si="4"/>
+        <v>x94</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>149</v>
+      </c>
+      <c r="B156" t="str">
+        <f t="shared" si="4"/>
+        <v>x95</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>150</v>
+      </c>
+      <c r="B157" t="str">
+        <f t="shared" si="4"/>
+        <v>x96</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>151</v>
+      </c>
+      <c r="B158" t="str">
+        <f t="shared" si="4"/>
+        <v>x97</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>152</v>
+      </c>
+      <c r="B159" t="str">
+        <f t="shared" si="4"/>
+        <v>x98</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>153</v>
+      </c>
+      <c r="B160" t="str">
+        <f t="shared" si="4"/>
+        <v>x99</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>154</v>
+      </c>
+      <c r="B161" t="str">
+        <f t="shared" si="4"/>
+        <v>x9A</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>155</v>
+      </c>
+      <c r="B162" t="str">
+        <f t="shared" si="4"/>
+        <v>x9B</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>156</v>
+      </c>
+      <c r="B163" t="str">
+        <f t="shared" si="4"/>
+        <v>x9C</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>157</v>
+      </c>
+      <c r="B164" t="str">
+        <f t="shared" si="4"/>
+        <v>x9D</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>158</v>
+      </c>
+      <c r="B165" t="str">
+        <f t="shared" si="4"/>
+        <v>x9E</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" s="47">
+        <v>159</v>
+      </c>
+      <c r="B166" s="47" t="str">
+        <f t="shared" si="4"/>
+        <v>x9F</v>
+      </c>
+      <c r="C166" s="47"/>
+      <c r="D166" s="47"/>
+      <c r="E166" s="47"/>
+      <c r="F166" s="48"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>160</v>
+      </c>
+      <c r="B167" t="str">
+        <f t="shared" si="4"/>
+        <v>xA0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>161</v>
+      </c>
+      <c r="B168" t="str">
+        <f t="shared" si="4"/>
+        <v>xA1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>162</v>
+      </c>
+      <c r="B169" t="str">
+        <f t="shared" si="4"/>
+        <v>xA2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>163</v>
+      </c>
+      <c r="B170" t="str">
+        <f t="shared" si="4"/>
+        <v>xA3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>164</v>
+      </c>
+      <c r="B171" t="str">
+        <f t="shared" si="4"/>
+        <v>xA4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>165</v>
+      </c>
+      <c r="B172" t="str">
+        <f t="shared" si="4"/>
+        <v>xA5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>166</v>
+      </c>
+      <c r="B173" t="str">
+        <f t="shared" si="4"/>
+        <v>xA6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>167</v>
+      </c>
+      <c r="B174" t="str">
+        <f t="shared" si="4"/>
+        <v>xA7</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>168</v>
+      </c>
+      <c r="B175" t="str">
+        <f t="shared" si="4"/>
+        <v>xA8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>169</v>
+      </c>
+      <c r="B176" t="str">
+        <f t="shared" si="4"/>
+        <v>xA9</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>170</v>
+      </c>
+      <c r="B177" t="str">
+        <f t="shared" si="4"/>
+        <v>xAA</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>171</v>
+      </c>
+      <c r="B178" t="str">
+        <f t="shared" si="4"/>
+        <v>xAB</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>172</v>
+      </c>
+      <c r="B179" t="str">
+        <f t="shared" si="4"/>
+        <v>xAC</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>173</v>
+      </c>
+      <c r="B180" t="str">
+        <f t="shared" si="4"/>
+        <v>xAD</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>174</v>
+      </c>
+      <c r="B181" t="str">
+        <f t="shared" si="4"/>
+        <v>xAE</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>175</v>
+      </c>
+      <c r="B182" t="str">
+        <f t="shared" si="4"/>
+        <v>xAF</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>176</v>
+      </c>
+      <c r="B183" t="str">
+        <f t="shared" si="4"/>
+        <v>xB0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>177</v>
+      </c>
+      <c r="B184" t="str">
+        <f t="shared" si="4"/>
+        <v>xB1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>178</v>
+      </c>
+      <c r="B185" t="str">
+        <f t="shared" si="4"/>
+        <v>xB2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>179</v>
+      </c>
+      <c r="B186" t="str">
+        <f t="shared" si="4"/>
+        <v>xB3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>180</v>
+      </c>
+      <c r="B187" t="str">
+        <f t="shared" si="4"/>
+        <v>xB4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>181</v>
+      </c>
+      <c r="B188" t="str">
+        <f t="shared" si="4"/>
+        <v>xB5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>182</v>
+      </c>
+      <c r="B189" t="str">
+        <f t="shared" si="4"/>
+        <v>xB6</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>183</v>
+      </c>
+      <c r="B190" t="str">
+        <f t="shared" si="4"/>
+        <v>xB7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>184</v>
+      </c>
+      <c r="B191" t="str">
+        <f t="shared" si="4"/>
+        <v>xB8</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>185</v>
+      </c>
+      <c r="B192" t="str">
+        <f t="shared" si="4"/>
+        <v>xB9</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>186</v>
+      </c>
+      <c r="B193" t="str">
+        <f t="shared" si="4"/>
+        <v>xBA</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>187</v>
+      </c>
+      <c r="B194" t="str">
+        <f t="shared" si="4"/>
+        <v>xBB</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>188</v>
+      </c>
+      <c r="B195" t="str">
+        <f t="shared" si="4"/>
+        <v>xBC</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>189</v>
+      </c>
+      <c r="B196" t="str">
+        <f t="shared" si="4"/>
+        <v>xBD</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>190</v>
+      </c>
+      <c r="B197" t="str">
+        <f t="shared" si="4"/>
+        <v>xBE</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>191</v>
+      </c>
+      <c r="B198" t="str">
+        <f t="shared" si="4"/>
+        <v>xBF</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>192</v>
+      </c>
+      <c r="B199" t="str">
+        <f t="shared" si="4"/>
+        <v>xC0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>193</v>
+      </c>
+      <c r="B200" t="str">
+        <f t="shared" si="4"/>
+        <v>xC1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>194</v>
+      </c>
+      <c r="B201" t="str">
+        <f t="shared" ref="B201:B264" si="5">"x" &amp; DEC2HEX(A201,2)</f>
+        <v>xC2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>195</v>
+      </c>
+      <c r="B202" t="str">
+        <f t="shared" si="5"/>
+        <v>xC3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>196</v>
+      </c>
+      <c r="B203" t="str">
+        <f t="shared" si="5"/>
+        <v>xC4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>197</v>
+      </c>
+      <c r="B204" t="str">
+        <f t="shared" si="5"/>
+        <v>xC5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>198</v>
+      </c>
+      <c r="B205" t="str">
+        <f t="shared" si="5"/>
+        <v>xC6</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>199</v>
+      </c>
+      <c r="B206" t="str">
+        <f t="shared" si="5"/>
+        <v>xC7</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>200</v>
+      </c>
+      <c r="B207" t="str">
+        <f t="shared" si="5"/>
+        <v>xC8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>201</v>
+      </c>
+      <c r="B208" t="str">
+        <f t="shared" si="5"/>
+        <v>xC9</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>202</v>
+      </c>
+      <c r="B209" t="str">
+        <f t="shared" si="5"/>
+        <v>xCA</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>203</v>
+      </c>
+      <c r="B210" t="str">
+        <f t="shared" si="5"/>
+        <v>xCB</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>204</v>
+      </c>
+      <c r="B211" t="str">
+        <f t="shared" si="5"/>
+        <v>xCC</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>205</v>
+      </c>
+      <c r="B212" t="str">
+        <f t="shared" si="5"/>
+        <v>xCD</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>206</v>
+      </c>
+      <c r="B213" t="str">
+        <f t="shared" si="5"/>
+        <v>xCE</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>207</v>
+      </c>
+      <c r="B214" t="str">
+        <f t="shared" si="5"/>
+        <v>xCF</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>208</v>
+      </c>
+      <c r="B215" t="str">
+        <f t="shared" si="5"/>
+        <v>xD0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>209</v>
+      </c>
+      <c r="B216" t="str">
+        <f t="shared" si="5"/>
+        <v>xD1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>210</v>
+      </c>
+      <c r="B217" t="str">
+        <f t="shared" si="5"/>
+        <v>xD2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>211</v>
+      </c>
+      <c r="B218" t="str">
+        <f t="shared" si="5"/>
+        <v>xD3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>212</v>
+      </c>
+      <c r="B219" t="str">
+        <f t="shared" si="5"/>
+        <v>xD4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>213</v>
+      </c>
+      <c r="B220" t="str">
+        <f t="shared" si="5"/>
+        <v>xD5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>214</v>
+      </c>
+      <c r="B221" t="str">
+        <f t="shared" si="5"/>
+        <v>xD6</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>215</v>
+      </c>
+      <c r="B222" t="str">
+        <f t="shared" si="5"/>
+        <v>xD7</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>216</v>
+      </c>
+      <c r="B223" t="str">
+        <f t="shared" si="5"/>
+        <v>xD8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>217</v>
+      </c>
+      <c r="B224" t="str">
+        <f t="shared" si="5"/>
+        <v>xD9</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>218</v>
+      </c>
+      <c r="B225" t="str">
+        <f t="shared" si="5"/>
+        <v>xDA</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>219</v>
+      </c>
+      <c r="B226" t="str">
+        <f t="shared" si="5"/>
+        <v>xDB</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>220</v>
+      </c>
+      <c r="B227" t="str">
+        <f t="shared" si="5"/>
+        <v>xDC</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>221</v>
+      </c>
+      <c r="B228" t="str">
+        <f t="shared" si="5"/>
+        <v>xDD</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>222</v>
+      </c>
+      <c r="B229" t="str">
+        <f t="shared" si="5"/>
+        <v>xDE</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>223</v>
+      </c>
+      <c r="B230" t="str">
+        <f t="shared" si="5"/>
+        <v>xDF</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>224</v>
+      </c>
+      <c r="B231" t="str">
+        <f t="shared" si="5"/>
+        <v>xE0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>225</v>
+      </c>
+      <c r="B232" t="str">
+        <f t="shared" si="5"/>
+        <v>xE1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>226</v>
+      </c>
+      <c r="B233" t="str">
+        <f t="shared" si="5"/>
+        <v>xE2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>227</v>
+      </c>
+      <c r="B234" t="str">
+        <f t="shared" si="5"/>
+        <v>xE3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>228</v>
+      </c>
+      <c r="B235" t="str">
+        <f t="shared" si="5"/>
+        <v>xE4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>229</v>
+      </c>
+      <c r="B236" t="str">
+        <f t="shared" si="5"/>
+        <v>xE5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>230</v>
+      </c>
+      <c r="B237" t="str">
+        <f t="shared" si="5"/>
+        <v>xE6</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>231</v>
+      </c>
+      <c r="B238" t="str">
+        <f t="shared" si="5"/>
+        <v>xE7</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>232</v>
+      </c>
+      <c r="B239" t="str">
+        <f t="shared" si="5"/>
+        <v>xE8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>233</v>
+      </c>
+      <c r="B240" t="str">
+        <f t="shared" si="5"/>
+        <v>xE9</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>234</v>
+      </c>
+      <c r="B241" t="str">
+        <f t="shared" si="5"/>
+        <v>xEA</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>235</v>
+      </c>
+      <c r="B242" t="str">
+        <f t="shared" si="5"/>
+        <v>xEB</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>236</v>
+      </c>
+      <c r="B243" t="str">
+        <f t="shared" si="5"/>
+        <v>xEC</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>237</v>
+      </c>
+      <c r="B244" t="str">
+        <f t="shared" si="5"/>
+        <v>xED</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>238</v>
+      </c>
+      <c r="B245" t="str">
+        <f t="shared" si="5"/>
+        <v>xEE</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>239</v>
+      </c>
+      <c r="B246" t="str">
+        <f t="shared" si="5"/>
+        <v>xEF</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>240</v>
+      </c>
+      <c r="B247" t="str">
+        <f t="shared" si="5"/>
+        <v>xF0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>241</v>
+      </c>
+      <c r="B248" t="str">
+        <f t="shared" si="5"/>
+        <v>xF1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>242</v>
+      </c>
+      <c r="B249" t="str">
+        <f t="shared" si="5"/>
+        <v>xF2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>243</v>
+      </c>
+      <c r="B250" t="str">
+        <f t="shared" si="5"/>
+        <v>xF3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>244</v>
+      </c>
+      <c r="B251" t="str">
+        <f t="shared" si="5"/>
+        <v>xF4</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>245</v>
+      </c>
+      <c r="B252" t="str">
+        <f t="shared" si="5"/>
+        <v>xF5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>246</v>
+      </c>
+      <c r="B253" t="str">
+        <f t="shared" si="5"/>
+        <v>xF6</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>247</v>
+      </c>
+      <c r="B254" t="str">
+        <f t="shared" si="5"/>
+        <v>xF7</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>248</v>
+      </c>
+      <c r="B255" t="str">
+        <f t="shared" si="5"/>
+        <v>xF8</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>249</v>
+      </c>
+      <c r="B256" t="str">
+        <f t="shared" si="5"/>
+        <v>xF9</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>250</v>
+      </c>
+      <c r="B257" t="str">
+        <f t="shared" si="5"/>
+        <v>xFA</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>251</v>
+      </c>
+      <c r="B258" t="str">
+        <f t="shared" si="5"/>
+        <v>xFB</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>252</v>
+      </c>
+      <c r="B259" t="str">
+        <f t="shared" si="5"/>
+        <v>xFC</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>253</v>
+      </c>
+      <c r="B260" t="str">
+        <f t="shared" si="5"/>
+        <v>xFD</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>254</v>
+      </c>
+      <c r="B261" t="str">
+        <f t="shared" si="5"/>
+        <v>xFE</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>255</v>
+      </c>
+      <c r="B262" t="str">
+        <f t="shared" si="5"/>
+        <v>xFF</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
compiles but untested with w/ flat beams
</commit_message>
<xml_diff>
--- a/doc/flower8-register-map.xlsx
+++ b/doc/flower8-register-map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryank\Documents\firmware\BEACON\FLOWER8-board-firmware\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryank\Documents\firmware\BEACON\dev\FLOWER8-board-firmware\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847262DA-EF74-48C1-B5E3-715E4BFA1076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288889D3-EABD-42CB-A0E7-BEDCF2FC3D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="228" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registers" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="242">
   <si>
     <t>Register Map</t>
   </si>
@@ -168,9 +168,6 @@
     <t>pick scaler to read</t>
   </si>
   <si>
-    <t>write something between 0x0 and 0xF, scaler to read pops up in read-register 3</t>
-  </si>
-  <si>
     <t>scaler_to_read</t>
   </si>
   <si>
@@ -510,9 +507,6 @@
     <t>read_only - event meta data [lowest 4 bits=trigger type, bit16=pps flag]</t>
   </si>
   <si>
-    <t>currently 32 scalers registers (12 bits per scaler, 2 scalers per 24 bit register)</t>
-  </si>
-  <si>
     <t>data in max_address location may not be useful</t>
   </si>
   <si>
@@ -669,9 +663,6 @@
     <t>lsb=1 is 100Hz, lsb=0 is 100mHz [default]</t>
   </si>
   <si>
-    <t>event metadata-&gt;trig</t>
-  </si>
-  <si>
     <t>read_only - event meta data -- low 8 bits latched trigger channels</t>
   </si>
   <si>
@@ -741,9 +732,6 @@
     <t>trigger mask - upper beams</t>
   </si>
   <si>
-    <t>trigger mask - lower bea,s</t>
-  </si>
-  <si>
     <t>beam mask in trigger [LSB-&gt;(num_beams-1-24)]</t>
   </si>
   <si>
@@ -751,6 +739,30 @@
   </si>
   <si>
     <t>beam 41 thresholds</t>
+  </si>
+  <si>
+    <t>event metadata-&gt;coinc_trig</t>
+  </si>
+  <si>
+    <t>event_metadata-&gt;phased_trig_low</t>
+  </si>
+  <si>
+    <t>read_only - event meta data - lower 24 beams</t>
+  </si>
+  <si>
+    <t>event_metadata-&gt;phased_trig_high</t>
+  </si>
+  <si>
+    <t>read_only - event meta data - upper 18 beams</t>
+  </si>
+  <si>
+    <t>318 scaler registers (12 bits per scaler, 2 scalers per 24 bit register)</t>
+  </si>
+  <si>
+    <t>write something between 0x0 and 0x1F, scaler to read pops up in read-register 3</t>
+  </si>
+  <si>
+    <t>trigger mask - lower beams</t>
   </si>
 </sst>
 </file>
@@ -962,7 +974,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1063,10 +1075,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1349,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1366,7 +1374,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -1394,7 +1402,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B4" s="46"/>
       <c r="C4" s="1"/>
@@ -1416,7 +1424,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
@@ -1439,10 +1447,10 @@
         <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7"/>
     </row>
@@ -1487,13 +1495,13 @@
         <v>x03</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1512,7 +1520,7 @@
         <v>35</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1544,13 +1552,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" t="s">
         <v>82</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1566,7 +1574,7 @@
         <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1579,7 +1587,7 @@
         <v>x08</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>16</v>
@@ -1595,7 +1603,7 @@
         <v>x09</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>16</v>
@@ -1611,16 +1619,16 @@
         <v>x0A</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1633,10 +1641,10 @@
         <v>x0B</v>
       </c>
       <c r="C18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -1653,10 +1661,10 @@
         <v>x0C</v>
       </c>
       <c r="C19" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -1673,10 +1681,10 @@
         <v>x0D</v>
       </c>
       <c r="C20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -1693,10 +1701,10 @@
         <v>x0E</v>
       </c>
       <c r="C21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -1713,16 +1721,16 @@
         <v>x0F</v>
       </c>
       <c r="C22" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" t="s">
         <v>155</v>
-      </c>
-      <c r="D22" t="s">
-        <v>156</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1735,10 +1743,13 @@
         <v>x10</v>
       </c>
       <c r="C23" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="D23" t="s">
-        <v>211</v>
+        <v>208</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
       </c>
       <c r="F23" s="13"/>
     </row>
@@ -1751,6 +1762,15 @@
         <f t="shared" si="0"/>
         <v>x11</v>
       </c>
+      <c r="C24" t="s">
+        <v>235</v>
+      </c>
+      <c r="D24" t="s">
+        <v>236</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
       <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1762,6 +1782,15 @@
         <f t="shared" si="0"/>
         <v>x12</v>
       </c>
+      <c r="C25" t="s">
+        <v>237</v>
+      </c>
+      <c r="D25" t="s">
+        <v>238</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
       <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1939,7 +1968,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D41" s="30"/>
       <c r="E41" s="30"/>
@@ -1955,13 +1984,13 @@
         <v>x23</v>
       </c>
       <c r="C42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1974,13 +2003,13 @@
         <v>x24</v>
       </c>
       <c r="C43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1993,13 +2022,13 @@
         <v>x25</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2012,13 +2041,13 @@
         <v>x26</v>
       </c>
       <c r="C45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="D45" t="s">
-        <v>62</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2031,16 +2060,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D46" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E46" s="37" t="s">
         <v>6</v>
       </c>
       <c r="F46" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2053,10 +2082,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" t="s">
         <v>117</v>
-      </c>
-      <c r="D47" t="s">
-        <v>118</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -2075,13 +2104,13 @@
         <v>42</v>
       </c>
       <c r="D48" t="s">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="E48" t="s">
         <v>6</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>43</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2097,7 +2126,7 @@
         <v>29</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E49" t="s">
         <v>6</v>
@@ -2126,13 +2155,13 @@
         <v>x2C</v>
       </c>
       <c r="C51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2145,13 +2174,13 @@
         <v>x2D</v>
       </c>
       <c r="C52" t="s">
+        <v>119</v>
+      </c>
+      <c r="D52" t="s">
+        <v>121</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="D52" t="s">
-        <v>122</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2174,10 +2203,10 @@
         <v>x2F</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>6</v>
@@ -2202,7 +2231,7 @@
         <v>41</v>
       </c>
       <c r="F55" s="35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2288,13 +2317,13 @@
         <v>21</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E63" t="s">
         <v>6</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2310,13 +2339,13 @@
         <v>22</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E64" t="s">
         <v>6</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2329,10 +2358,10 @@
         <v>x3A</v>
       </c>
       <c r="C65" t="s">
+        <v>135</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="E65" t="s">
         <v>6</v>
@@ -2348,10 +2377,10 @@
         <v>x3B</v>
       </c>
       <c r="C66" t="s">
+        <v>132</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="E66" t="s">
         <v>6</v>
@@ -2367,10 +2396,10 @@
         <v>x3C</v>
       </c>
       <c r="C67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E67" t="s">
         <v>6</v>
@@ -2386,16 +2415,16 @@
         <v>x3D</v>
       </c>
       <c r="C68" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E68" t="s">
         <v>6</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2409,7 +2438,7 @@
       </c>
       <c r="D69" s="3"/>
       <c r="F69" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2455,7 +2484,7 @@
         <v>10</v>
       </c>
       <c r="D72" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E72" t="s">
         <v>7</v>
@@ -2471,13 +2500,13 @@
         <v>x42</v>
       </c>
       <c r="C73" t="s">
+        <v>137</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="F73" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2501,16 +2530,16 @@
         <v>x44</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F75" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2526,13 +2555,13 @@
         <v>24</v>
       </c>
       <c r="D76" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E76" t="s">
         <v>7</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2565,7 +2594,7 @@
         <v>7</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2587,7 +2616,7 @@
         <v>7</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2623,16 +2652,16 @@
         <v>x4B</v>
       </c>
       <c r="C82" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D82" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="E82" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="F82" s="36" t="s">
         <v>113</v>
-      </c>
-      <c r="D82" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="E82" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="F82" s="36" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -2648,13 +2677,13 @@
         <v>34</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E83" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -2667,16 +2696,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E84" t="s">
         <v>7</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -2698,7 +2727,7 @@
         <v>7</v>
       </c>
       <c r="F85" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -2723,16 +2752,16 @@
         <f t="shared" si="2"/>
         <v>x50</v>
       </c>
-      <c r="C87" s="32" t="s">
-        <v>234</v>
-      </c>
-      <c r="D87" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="E87" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="F87" s="33" t="s">
+      <c r="C87" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D87" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="E87" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F87" s="18" t="s">
         <v>32</v>
       </c>
       <c r="G87" s="6"/>
@@ -2746,16 +2775,16 @@
         <f t="shared" si="2"/>
         <v>x51</v>
       </c>
-      <c r="C88" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="D88" s="33" t="s">
+      <c r="C88" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="D88" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E88" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="F88" s="33"/>
+      <c r="E88" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F88" s="18"/>
       <c r="G88" s="6"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -2768,16 +2797,16 @@
         <v>x52</v>
       </c>
       <c r="C89" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D89" s="33" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E89" s="32" t="s">
         <v>7</v>
       </c>
       <c r="F89" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G89" s="6"/>
     </row>
@@ -2791,19 +2820,19 @@
         <v>x53</v>
       </c>
       <c r="C90" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D90" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="E90" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="F90" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="E90" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="F90" s="33" t="s">
-        <v>124</v>
-      </c>
       <c r="G90" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -2849,16 +2878,16 @@
         <v>x56</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="94" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2871,10 +2900,10 @@
         <v>x57</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>7</v>
@@ -2891,10 +2920,10 @@
         <v>x58</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>7</v>
@@ -2911,10 +2940,10 @@
         <v>x59</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>7</v>
@@ -2931,10 +2960,10 @@
         <v>x5A</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>7</v>
@@ -2951,10 +2980,10 @@
         <v>x5B</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>7</v>
@@ -2971,10 +3000,10 @@
         <v>x5C</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>7</v>
@@ -2991,10 +3020,10 @@
         <v>x5D</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>7</v>
@@ -3011,10 +3040,10 @@
         <v>x5E</v>
       </c>
       <c r="C101" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E101" t="s">
         <v>11</v>
@@ -3030,13 +3059,13 @@
         <v>x5F</v>
       </c>
       <c r="C102" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="F102" s="5"/>
     </row>
@@ -3050,16 +3079,16 @@
         <v>x60</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="104" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3072,10 +3101,10 @@
         <v>x61</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>7</v>
@@ -3092,13 +3121,13 @@
         <v>x62</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3111,10 +3140,10 @@
         <v>x63</v>
       </c>
       <c r="C106" s="41" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D106" s="42" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E106" s="41" t="s">
         <v>7</v>
@@ -3153,13 +3182,13 @@
         <v>x66</v>
       </c>
       <c r="D109" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E109" s="22" t="s">
         <v>6</v>
       </c>
       <c r="F109" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="110" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3172,13 +3201,13 @@
         <v>x67</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D110" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F110" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="111" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3191,10 +3220,10 @@
         <v>x68</v>
       </c>
       <c r="C111" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F111" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="112" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3207,10 +3236,10 @@
         <v>x69</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F112" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="113" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3223,10 +3252,10 @@
         <v>x6A</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F113" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="114" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3239,11 +3268,11 @@
         <v>x6B</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D114" s="43"/>
       <c r="F114" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3256,16 +3285,16 @@
         <v>x6C</v>
       </c>
       <c r="C115" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D115" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E115" t="s">
         <v>6</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3278,7 +3307,7 @@
         <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D116" t="s">
         <v>18</v>
@@ -3287,7 +3316,7 @@
         <v>19</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="117" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3300,13 +3329,13 @@
         <v>x6E</v>
       </c>
       <c r="C117" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D117" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F117" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="118" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3319,13 +3348,13 @@
         <v>x6F</v>
       </c>
       <c r="C118" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D118" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F118" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="119" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3338,13 +3367,13 @@
         <v>x70</v>
       </c>
       <c r="C119" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D119" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F119" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="120" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3357,13 +3386,13 @@
         <v>x71</v>
       </c>
       <c r="C120" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D120" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F120" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="121" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3376,13 +3405,13 @@
         <v>x72</v>
       </c>
       <c r="C121" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D121" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="D121" s="19" t="s">
-        <v>98</v>
-      </c>
       <c r="F121" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="122" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3395,13 +3424,13 @@
         <v>x73</v>
       </c>
       <c r="C122" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D122" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F122" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="123" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3414,13 +3443,13 @@
         <v>x74</v>
       </c>
       <c r="C123" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D123" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F123" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="124" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3433,13 +3462,13 @@
         <v>x75</v>
       </c>
       <c r="C124" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D124" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D124" s="19" t="s">
-        <v>100</v>
-      </c>
       <c r="F124" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="125" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3452,13 +3481,13 @@
         <v>x76</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D125" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F125" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="126" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3471,13 +3500,13 @@
         <v>x77</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D126" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F126" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="127" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3490,10 +3519,10 @@
         <v>x78</v>
       </c>
       <c r="C127" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F127" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3506,13 +3535,13 @@
         <v>x79</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D128" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F128" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3535,10 +3564,10 @@
         <v>x7B</v>
       </c>
       <c r="C130" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F130" s="27" t="s">
         <v>129</v>
-      </c>
-      <c r="F130" s="27" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.3">
@@ -3551,10 +3580,10 @@
         <v>x7C</v>
       </c>
       <c r="C131" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F131" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3579,10 +3608,10 @@
         <v>x7E</v>
       </c>
       <c r="C133" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D133" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E133" t="s">
         <v>7</v>
@@ -3601,13 +3630,13 @@
         <v>5</v>
       </c>
       <c r="D134" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E134" s="37" t="s">
         <v>7</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3628,13 +3657,13 @@
         <v>x81</v>
       </c>
       <c r="C136" s="10" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D136" s="10" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E136" s="10" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F136" s="44"/>
     </row>
@@ -3773,7 +3802,7 @@
         <v>x90</v>
       </c>
       <c r="C151" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -3857,7 +3886,7 @@
         <v>x99</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>154</v>
       </c>
@@ -3866,7 +3895,7 @@
         <v>x9A</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>155</v>
       </c>
@@ -3875,7 +3904,7 @@
         <v>x9B</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>156</v>
       </c>
@@ -3884,7 +3913,7 @@
         <v>x9C</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>157</v>
       </c>
@@ -3893,7 +3922,7 @@
         <v>x9D</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>158</v>
       </c>
@@ -3902,20 +3931,16 @@
         <v>x9E</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A166" s="48">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166">
         <v>159</v>
       </c>
-      <c r="B166" s="48" t="str">
+      <c r="B166" t="str">
         <f t="shared" si="4"/>
         <v>x9F</v>
       </c>
-      <c r="C166" s="48"/>
-      <c r="D166" s="48"/>
-      <c r="E166" s="48"/>
-      <c r="F166" s="49"/>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>160</v>
       </c>
@@ -3924,7 +3949,7 @@
         <v>xA0</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>161</v>
       </c>
@@ -3933,7 +3958,7 @@
         <v>xA1</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>162</v>
       </c>
@@ -3942,7 +3967,7 @@
         <v>xA2</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>163</v>
       </c>
@@ -3951,7 +3976,7 @@
         <v>xA3</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>164</v>
       </c>
@@ -3960,7 +3985,7 @@
         <v>xA4</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>165</v>
       </c>
@@ -3969,7 +3994,7 @@
         <v>xA5</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>166</v>
       </c>
@@ -3978,7 +4003,7 @@
         <v>xA6</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>167</v>
       </c>
@@ -3987,7 +4012,7 @@
         <v>xA7</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>168</v>
       </c>
@@ -3996,7 +4021,7 @@
         <v>xA8</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>169</v>
       </c>
@@ -4023,7 +4048,7 @@
         <v>xAB</v>
       </c>
       <c r="C178" s="45" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D178" s="45"/>
     </row>
@@ -4815,19 +4840,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4838,10 +4863,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -4853,10 +4878,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -4868,10 +4893,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -4883,10 +4908,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -4898,10 +4923,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -4913,10 +4938,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -4928,10 +4953,10 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -4943,10 +4968,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -4958,10 +4983,10 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -4973,10 +4998,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -4988,10 +5013,10 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -5003,10 +5028,10 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -5018,10 +5043,10 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -5033,10 +5058,10 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -5048,10 +5073,10 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -5063,10 +5088,10 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -5078,10 +5103,10 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -5093,10 +5118,10 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -5108,10 +5133,10 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D20" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -5123,10 +5148,10 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -5138,10 +5163,10 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D22" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -5153,10 +5178,10 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -5168,10 +5193,10 @@
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -5183,10 +5208,10 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D25" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -5198,10 +5223,10 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -5213,10 +5238,10 @@
         <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D27" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -5228,10 +5253,10 @@
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -5243,10 +5268,10 @@
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D29" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -5258,10 +5283,10 @@
         <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D30" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -5273,10 +5298,10 @@
         <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -5288,10 +5313,10 @@
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D32" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -5303,10 +5328,10 @@
         <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D33" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -5318,10 +5343,10 @@
         <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D34" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -5333,10 +5358,10 @@
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -5348,10 +5373,10 @@
         <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D36" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -5363,10 +5388,10 @@
         <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D37" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -5378,10 +5403,10 @@
         <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -5393,10 +5418,10 @@
         <v>18</v>
       </c>
       <c r="C39" t="s">
+        <v>195</v>
+      </c>
+      <c r="D39" t="s">
         <v>197</v>
-      </c>
-      <c r="D39" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -5408,10 +5433,10 @@
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D40" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -5423,10 +5448,10 @@
         <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -5438,13 +5463,13 @@
         <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D42" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E42" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -5456,10 +5481,10 @@
         <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D43" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -5471,10 +5496,10 @@
         <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D44" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -5486,10 +5511,10 @@
         <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -5501,10 +5526,10 @@
         <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D46" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -5516,10 +5541,10 @@
         <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -5531,10 +5556,10 @@
         <v>23</v>
       </c>
       <c r="C48" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D48" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -5546,10 +5571,10 @@
         <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D49" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -5561,10 +5586,10 @@
         <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D50" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -5576,10 +5601,10 @@
         <v>24</v>
       </c>
       <c r="C51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D51" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -5591,10 +5616,10 @@
         <v>25</v>
       </c>
       <c r="C52" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D52" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -5606,10 +5631,10 @@
         <v>25</v>
       </c>
       <c r="C53" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D53" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -5621,10 +5646,10 @@
         <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D54" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -5636,10 +5661,10 @@
         <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D55" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -5651,10 +5676,10 @@
         <v>27</v>
       </c>
       <c r="C56" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D56" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -5666,10 +5691,10 @@
         <v>27</v>
       </c>
       <c r="C57" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D57" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -5681,10 +5706,10 @@
         <v>28</v>
       </c>
       <c r="C58" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D58" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -5696,10 +5721,10 @@
         <v>28</v>
       </c>
       <c r="C59" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D59" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -5711,10 +5736,10 @@
         <v>29</v>
       </c>
       <c r="C60" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" t="s">
         <v>198</v>
-      </c>
-      <c r="D60" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -5726,10 +5751,10 @@
         <v>29</v>
       </c>
       <c r="C61" t="s">
+        <v>196</v>
+      </c>
+      <c r="D61" t="s">
         <v>198</v>
-      </c>
-      <c r="D61" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -5741,7 +5766,7 @@
         <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -5753,7 +5778,7 @@
         <v>30</v>
       </c>
       <c r="C63" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -5764,7 +5789,7 @@
         <v>31</v>
       </c>
       <c r="C64" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -5775,7 +5800,7 @@
         <v>31</v>
       </c>
       <c r="C65" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -5783,7 +5808,7 @@
         <v>32</v>
       </c>
       <c r="C66" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -5791,7 +5816,7 @@
         <v>33</v>
       </c>
       <c r="C67" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
band-aid the ADC bug, fix small things, phased trigger tested
</commit_message>
<xml_diff>
--- a/doc/flower8-register-map.xlsx
+++ b/doc/flower8-register-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryank\Documents\firmware\BEACON\dev\FLOWER8-board-firmware\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D403EF-EDAA-4700-AE43-F4A9B7F81900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703FE3F3-F35E-4385-95AE-397F92C48CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="228" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registers" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="287">
   <si>
     <t>Register Map</t>
   </si>
@@ -636,9 +636,6 @@
     <t>100Hz</t>
   </si>
   <si>
-    <t>1Hz scaler update counter</t>
-  </si>
-  <si>
     <t>all 12 bits -- 2 scalers per scaler adr</t>
   </si>
   <si>
@@ -763,6 +760,144 @@
   </si>
   <si>
     <t>trigger mask - lower beams</t>
+  </si>
+  <si>
+    <t>pps</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>something</t>
+  </si>
+  <si>
+    <t>Phased Trigger</t>
+  </si>
+  <si>
+    <t>Beam 0 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 1 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 2 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 3 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 4 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 5 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 6 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 7 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 8 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 9 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 10 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 11 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 12 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 13 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 14 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 15 Trigger</t>
+  </si>
+  <si>
+    <t>Phased Servo</t>
+  </si>
+  <si>
+    <t>Beam 0 Servo</t>
+  </si>
+  <si>
+    <t>Beam 1 Servo</t>
+  </si>
+  <si>
+    <t>Beam 2 Servo</t>
+  </si>
+  <si>
+    <t>Beam 3 Servo</t>
+  </si>
+  <si>
+    <t>Beam 4 Servo</t>
+  </si>
+  <si>
+    <t>Beam 5 Servo</t>
+  </si>
+  <si>
+    <t>Beam 6 Servo</t>
+  </si>
+  <si>
+    <t>Beam 7 Servo</t>
+  </si>
+  <si>
+    <t>Beam 8 Servo</t>
+  </si>
+  <si>
+    <t>Beam 9 Servo</t>
+  </si>
+  <si>
+    <t>Beam 10 Servo</t>
+  </si>
+  <si>
+    <t>Beam 11 Servo</t>
+  </si>
+  <si>
+    <t>Beam 12 Servo</t>
+  </si>
+  <si>
+    <t>Beam 13 Servo</t>
+  </si>
+  <si>
+    <t>Beam 14 Servo</t>
+  </si>
+  <si>
+    <t>Beam 15 Servo</t>
+  </si>
+  <si>
+    <t>1Hz Gated</t>
+  </si>
+  <si>
+    <t>Beam 16 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 17 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 18 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 19 Trigger</t>
+  </si>
+  <si>
+    <t>Beam 16 Servo</t>
+  </si>
+  <si>
+    <t>Beam 17 Servo</t>
+  </si>
+  <si>
+    <t>Beam 18 Servo</t>
+  </si>
+  <si>
+    <t>Beam 19 Servo</t>
   </si>
 </sst>
 </file>
@@ -974,7 +1109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1075,7 +1210,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1358,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="C140" sqref="C140"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1403,7 +1537,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4" s="46"/>
       <c r="C4" s="1"/>
@@ -1662,7 +1796,7 @@
         <v>x0C</v>
       </c>
       <c r="C19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D19" t="s">
         <v>45</v>
@@ -1744,10 +1878,10 @@
         <v>x10</v>
       </c>
       <c r="C23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
@@ -1764,10 +1898,10 @@
         <v>x11</v>
       </c>
       <c r="C24" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" t="s">
         <v>235</v>
-      </c>
-      <c r="D24" t="s">
-        <v>236</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
@@ -1784,10 +1918,10 @@
         <v>x12</v>
       </c>
       <c r="C25" t="s">
+        <v>236</v>
+      </c>
+      <c r="D25" t="s">
         <v>237</v>
-      </c>
-      <c r="D25" t="s">
-        <v>238</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
@@ -2105,13 +2239,13 @@
         <v>42</v>
       </c>
       <c r="D48" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E48" t="s">
         <v>6</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2204,10 +2338,10 @@
         <v>x2F</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>6</v>
@@ -2419,13 +2553,13 @@
         <v>144</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E68" t="s">
         <v>6</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2754,10 +2888,10 @@
         <v>x50</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D87" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>49</v>
@@ -2777,7 +2911,7 @@
         <v>x51</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D88" s="18" t="s">
         <v>33</v>
@@ -2801,7 +2935,7 @@
         <v>111</v>
       </c>
       <c r="D89" s="33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E89" s="32" t="s">
         <v>7</v>
@@ -2833,7 +2967,7 @@
         <v>123</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -2879,16 +3013,16 @@
         <v>x56</v>
       </c>
       <c r="C93" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D93" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>219</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="94" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2901,10 +3035,10 @@
         <v>x57</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>7</v>
@@ -2921,10 +3055,10 @@
         <v>x58</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>7</v>
@@ -2941,10 +3075,10 @@
         <v>x59</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>7</v>
@@ -2961,10 +3095,10 @@
         <v>x5A</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>7</v>
@@ -2981,10 +3115,10 @@
         <v>x5B</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>7</v>
@@ -3001,10 +3135,10 @@
         <v>x5C</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>7</v>
@@ -3021,10 +3155,10 @@
         <v>x5D</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>7</v>
@@ -3089,7 +3223,7 @@
         <v>11</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3122,13 +3256,13 @@
         <v>x62</v>
       </c>
       <c r="C105" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D105" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D105" s="5" t="s">
+      <c r="E105" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3650,13 +3784,13 @@
         <v>x80</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D135" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F135" s="44"/>
     </row>
@@ -3665,7 +3799,7 @@
         <f t="shared" si="3"/>
         <v>129</v>
       </c>
-      <c r="B136" s="48" t="str">
+      <c r="B136" t="str">
         <f>"x" &amp; DEC2HEX(A136,2)</f>
         <v>x81</v>
       </c>
@@ -3805,7 +3939,7 @@
         <v>x90</v>
       </c>
       <c r="C151" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -4042,7 +4176,7 @@
         <v>xAA</v>
       </c>
       <c r="C177" s="45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D177" s="45"/>
     </row>
@@ -4825,11 +4959,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4855,51 +4989,45 @@
         <v>174</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
+        <f>FLOOR(A2/2,1)</f>
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
       </c>
       <c r="B3">
+        <f>FLOOR(A3/2,1)</f>
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A63" si="0">A3+1</f>
+        <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4">
+        <f>FLOOR(A4/2,1)</f>
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -4908,13 +5036,11 @@
         <v>3</v>
       </c>
       <c r="B5">
+        <f>FLOOR(A5/2,1)</f>
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D5" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -4923,13 +5049,11 @@
         <v>4</v>
       </c>
       <c r="B6">
+        <f t="shared" ref="B6:B69" si="1">FLOOR(A6/2,1)</f>
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
-      </c>
-      <c r="D6" t="s">
-        <v>176</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -4938,13 +5062,11 @@
         <v>5</v>
       </c>
       <c r="B7">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>183</v>
-      </c>
-      <c r="D7" t="s">
-        <v>176</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -4953,10 +5075,11 @@
         <v>6</v>
       </c>
       <c r="B8">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D8" t="s">
         <v>176</v>
@@ -4968,10 +5091,11 @@
         <v>7</v>
       </c>
       <c r="B9">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D9" t="s">
         <v>176</v>
@@ -4983,10 +5107,11 @@
         <v>8</v>
       </c>
       <c r="B10">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D10" t="s">
         <v>176</v>
@@ -4998,10 +5123,11 @@
         <v>9</v>
       </c>
       <c r="B11">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D11" t="s">
         <v>176</v>
@@ -5013,10 +5139,11 @@
         <v>10</v>
       </c>
       <c r="B12">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D12" t="s">
         <v>176</v>
@@ -5028,10 +5155,11 @@
         <v>11</v>
       </c>
       <c r="B13">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D13" t="s">
         <v>176</v>
@@ -5043,10 +5171,11 @@
         <v>12</v>
       </c>
       <c r="B14">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D14" t="s">
         <v>176</v>
@@ -5058,10 +5187,11 @@
         <v>13</v>
       </c>
       <c r="B15">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D15" t="s">
         <v>176</v>
@@ -5073,10 +5203,11 @@
         <v>14</v>
       </c>
       <c r="B16">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D16" t="s">
         <v>176</v>
@@ -5088,10 +5219,11 @@
         <v>15</v>
       </c>
       <c r="B17">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D17" t="s">
         <v>176</v>
@@ -5103,10 +5235,11 @@
         <v>16</v>
       </c>
       <c r="B18">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D18" t="s">
         <v>176</v>
@@ -5118,10 +5251,11 @@
         <v>17</v>
       </c>
       <c r="B19">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D19" t="s">
         <v>176</v>
@@ -5133,10 +5267,11 @@
         <v>18</v>
       </c>
       <c r="B20">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D20" t="s">
         <v>176</v>
@@ -5148,10 +5283,11 @@
         <v>19</v>
       </c>
       <c r="B21">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D21" t="s">
         <v>176</v>
@@ -5163,13 +5299,14 @@
         <v>20</v>
       </c>
       <c r="B22">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="D22" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -5178,13 +5315,14 @@
         <v>21</v>
       </c>
       <c r="B23">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="D23" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -5193,13 +5331,14 @@
         <v>22</v>
       </c>
       <c r="B24">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="D24" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -5208,13 +5347,14 @@
         <v>23</v>
       </c>
       <c r="B25">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="D25" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -5223,13 +5363,14 @@
         <v>24</v>
       </c>
       <c r="B26">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="D26" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -5238,13 +5379,14 @@
         <v>25</v>
       </c>
       <c r="B27">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="D27" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -5253,10 +5395,11 @@
         <v>26</v>
       </c>
       <c r="B28">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D28" t="s">
         <v>197</v>
@@ -5268,10 +5411,11 @@
         <v>27</v>
       </c>
       <c r="B29">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D29" t="s">
         <v>197</v>
@@ -5283,10 +5427,11 @@
         <v>28</v>
       </c>
       <c r="B30">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D30" t="s">
         <v>197</v>
@@ -5298,10 +5443,11 @@
         <v>29</v>
       </c>
       <c r="B31">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D31" t="s">
         <v>197</v>
@@ -5313,10 +5459,11 @@
         <v>30</v>
       </c>
       <c r="B32">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D32" t="s">
         <v>197</v>
@@ -5328,10 +5475,11 @@
         <v>31</v>
       </c>
       <c r="B33">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D33" t="s">
         <v>197</v>
@@ -5343,10 +5491,11 @@
         <v>32</v>
       </c>
       <c r="B34">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D34" t="s">
         <v>197</v>
@@ -5358,10 +5507,11 @@
         <v>33</v>
       </c>
       <c r="B35">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D35" t="s">
         <v>197</v>
@@ -5373,10 +5523,11 @@
         <v>34</v>
       </c>
       <c r="B36">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D36" t="s">
         <v>197</v>
@@ -5388,10 +5539,11 @@
         <v>35</v>
       </c>
       <c r="B37">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D37" t="s">
         <v>197</v>
@@ -5403,10 +5555,11 @@
         <v>36</v>
       </c>
       <c r="B38">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D38" t="s">
         <v>197</v>
@@ -5418,10 +5571,11 @@
         <v>37</v>
       </c>
       <c r="B39">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D39" t="s">
         <v>197</v>
@@ -5433,10 +5587,11 @@
         <v>38</v>
       </c>
       <c r="B40">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D40" t="s">
         <v>197</v>
@@ -5448,10 +5603,11 @@
         <v>39</v>
       </c>
       <c r="B41">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D41" t="s">
         <v>197</v>
@@ -5463,16 +5619,14 @@
         <v>40</v>
       </c>
       <c r="B42">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="D42" t="s">
-        <v>198</v>
-      </c>
-      <c r="E42" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -5481,13 +5635,14 @@
         <v>41</v>
       </c>
       <c r="B43">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="D43" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -5496,13 +5651,14 @@
         <v>42</v>
       </c>
       <c r="B44">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="D44" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -5511,13 +5667,17 @@
         <v>43</v>
       </c>
       <c r="B45">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="D45" t="s">
-        <v>198</v>
+        <v>197</v>
+      </c>
+      <c r="E45" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -5526,13 +5686,14 @@
         <v>44</v>
       </c>
       <c r="B46">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="D46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -5541,13 +5702,14 @@
         <v>45</v>
       </c>
       <c r="B47">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="D47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -5556,10 +5718,11 @@
         <v>46</v>
       </c>
       <c r="B48">
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="C48" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D48" t="s">
         <v>198</v>
@@ -5571,10 +5734,11 @@
         <v>47</v>
       </c>
       <c r="B49">
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D49" t="s">
         <v>198</v>
@@ -5586,10 +5750,11 @@
         <v>48</v>
       </c>
       <c r="B50">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D50" t="s">
         <v>198</v>
@@ -5601,10 +5766,11 @@
         <v>49</v>
       </c>
       <c r="B51">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C51" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D51" t="s">
         <v>198</v>
@@ -5616,10 +5782,11 @@
         <v>50</v>
       </c>
       <c r="B52">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="C52" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D52" t="s">
         <v>198</v>
@@ -5631,10 +5798,11 @@
         <v>51</v>
       </c>
       <c r="B53">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="C53" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D53" t="s">
         <v>198</v>
@@ -5646,10 +5814,11 @@
         <v>52</v>
       </c>
       <c r="B54">
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D54" t="s">
         <v>198</v>
@@ -5661,10 +5830,11 @@
         <v>53</v>
       </c>
       <c r="B55">
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D55" t="s">
         <v>198</v>
@@ -5676,10 +5846,11 @@
         <v>54</v>
       </c>
       <c r="B56">
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C56" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D56" t="s">
         <v>198</v>
@@ -5691,10 +5862,11 @@
         <v>55</v>
       </c>
       <c r="B57">
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C57" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D57" t="s">
         <v>198</v>
@@ -5706,10 +5878,11 @@
         <v>56</v>
       </c>
       <c r="B58">
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C58" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D58" t="s">
         <v>198</v>
@@ -5721,10 +5894,11 @@
         <v>57</v>
       </c>
       <c r="B59">
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C59" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D59" t="s">
         <v>198</v>
@@ -5736,10 +5910,11 @@
         <v>58</v>
       </c>
       <c r="B60">
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C60" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D60" t="s">
         <v>198</v>
@@ -5751,10 +5926,11 @@
         <v>59</v>
       </c>
       <c r="B61">
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C61" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D61" t="s">
         <v>198</v>
@@ -5766,10 +5942,14 @@
         <v>60</v>
       </c>
       <c r="B62">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>196</v>
+        <v>192</v>
+      </c>
+      <c r="D62" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -5778,48 +5958,2062 @@
         <v>61</v>
       </c>
       <c r="B63">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C63" t="s">
-        <v>196</v>
+        <v>193</v>
+      </c>
+      <c r="D63" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="B64">
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C64" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+      <c r="D64" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="B65">
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C65" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="D65" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
       <c r="B66">
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="C66" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+      <c r="D66" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
       <c r="B67">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="C67" t="s">
+        <v>245</v>
+      </c>
+      <c r="D67" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <f t="shared" ref="A68:A131" si="2">A67+1</f>
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="C67" t="s">
-        <v>202</v>
+      <c r="C68" t="s">
+        <v>246</v>
+      </c>
+      <c r="D68" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="C69" t="s">
+        <v>247</v>
+      </c>
+      <c r="D69" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <f t="shared" ref="B70:B133" si="3">FLOOR(A70/2,1)</f>
+        <v>34</v>
+      </c>
+      <c r="C70" t="s">
+        <v>248</v>
+      </c>
+      <c r="D70" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="C71" t="s">
+        <v>249</v>
+      </c>
+      <c r="D71" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="C72" t="s">
+        <v>250</v>
+      </c>
+      <c r="D72" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="C73" t="s">
+        <v>251</v>
+      </c>
+      <c r="D73" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="C74" t="s">
+        <v>252</v>
+      </c>
+      <c r="D74" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="C75" t="s">
+        <v>253</v>
+      </c>
+      <c r="D75" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="C76" t="s">
+        <v>254</v>
+      </c>
+      <c r="D76" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="C77" t="s">
+        <v>255</v>
+      </c>
+      <c r="D77" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="C78" t="s">
+        <v>256</v>
+      </c>
+      <c r="D78" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <f t="shared" si="2"/>
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="C79" t="s">
+        <v>257</v>
+      </c>
+      <c r="D79" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="C80" t="s">
+        <v>258</v>
+      </c>
+      <c r="D80" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="C81" t="s">
+        <v>259</v>
+      </c>
+      <c r="D81" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="C82" t="s">
+        <v>260</v>
+      </c>
+      <c r="D82" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="C83" t="s">
+        <v>279</v>
+      </c>
+      <c r="D83" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="C84" t="s">
+        <v>280</v>
+      </c>
+      <c r="D84" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <f t="shared" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="C85" t="s">
+        <v>281</v>
+      </c>
+      <c r="D85" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="C86" t="s">
+        <v>282</v>
+      </c>
+      <c r="D86" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="C87" t="s">
+        <v>261</v>
+      </c>
+      <c r="D87" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="C88" t="s">
+        <v>262</v>
+      </c>
+      <c r="D88" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="C89" t="s">
+        <v>263</v>
+      </c>
+      <c r="D89" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="C90" t="s">
+        <v>264</v>
+      </c>
+      <c r="D90" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="C91" t="s">
+        <v>265</v>
+      </c>
+      <c r="D91" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="C92" t="s">
+        <v>266</v>
+      </c>
+      <c r="D92" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="C93" t="s">
+        <v>267</v>
+      </c>
+      <c r="D93" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="C94" t="s">
+        <v>268</v>
+      </c>
+      <c r="D94" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <f t="shared" si="2"/>
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="C95" t="s">
+        <v>269</v>
+      </c>
+      <c r="D95" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="C96" t="s">
+        <v>270</v>
+      </c>
+      <c r="D96" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="C97" t="s">
+        <v>271</v>
+      </c>
+      <c r="D97" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="C98" t="s">
+        <v>272</v>
+      </c>
+      <c r="D98" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="C99" t="s">
+        <v>273</v>
+      </c>
+      <c r="D99" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="C100" t="s">
+        <v>274</v>
+      </c>
+      <c r="D100" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="C101" t="s">
+        <v>275</v>
+      </c>
+      <c r="D101" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="C102" t="s">
+        <v>276</v>
+      </c>
+      <c r="D102" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="C103" t="s">
+        <v>277</v>
+      </c>
+      <c r="D103" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="C104" t="s">
+        <v>283</v>
+      </c>
+      <c r="D104" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="C105" t="s">
+        <v>284</v>
+      </c>
+      <c r="D105" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="C106" t="s">
+        <v>285</v>
+      </c>
+      <c r="D106" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="C107" t="s">
+        <v>286</v>
+      </c>
+      <c r="D107" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="C108" t="s">
+        <v>244</v>
+      </c>
+      <c r="D108" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="C109" t="s">
+        <v>245</v>
+      </c>
+      <c r="D109" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="C110" t="s">
+        <v>246</v>
+      </c>
+      <c r="D110" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <f t="shared" si="2"/>
+        <v>109</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="C111" t="s">
+        <v>247</v>
+      </c>
+      <c r="D111" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="C112" t="s">
+        <v>248</v>
+      </c>
+      <c r="D112" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="B113">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="C113" t="s">
+        <v>249</v>
+      </c>
+      <c r="D113" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="C114" t="s">
+        <v>250</v>
+      </c>
+      <c r="D114" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+      <c r="B115">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="C115" t="s">
+        <v>251</v>
+      </c>
+      <c r="D115" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="C116" t="s">
+        <v>252</v>
+      </c>
+      <c r="D116" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="C117" t="s">
+        <v>253</v>
+      </c>
+      <c r="D117" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="C118" t="s">
+        <v>254</v>
+      </c>
+      <c r="D118" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="B119">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="C119" t="s">
+        <v>255</v>
+      </c>
+      <c r="D119" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="C120" t="s">
+        <v>256</v>
+      </c>
+      <c r="D120" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="C121" t="s">
+        <v>257</v>
+      </c>
+      <c r="D121" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="B122">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="C122" t="s">
+        <v>258</v>
+      </c>
+      <c r="D122" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="B123">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="C123" t="s">
+        <v>259</v>
+      </c>
+      <c r="D123" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <f t="shared" si="2"/>
+        <v>122</v>
+      </c>
+      <c r="B124">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="C124" t="s">
+        <v>260</v>
+      </c>
+      <c r="D124" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <f t="shared" si="2"/>
+        <v>123</v>
+      </c>
+      <c r="B125">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="C125" t="s">
+        <v>279</v>
+      </c>
+      <c r="D125" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="B126">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="C126" t="s">
+        <v>280</v>
+      </c>
+      <c r="D126" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+      <c r="B127">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="C127" t="s">
+        <v>281</v>
+      </c>
+      <c r="D127" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+      <c r="B128">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="C128" t="s">
+        <v>282</v>
+      </c>
+      <c r="D128" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <f t="shared" si="2"/>
+        <v>127</v>
+      </c>
+      <c r="B129">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="C129" t="s">
+        <v>261</v>
+      </c>
+      <c r="D129" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="B130">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="C130" t="s">
+        <v>262</v>
+      </c>
+      <c r="D130" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <f t="shared" si="2"/>
+        <v>129</v>
+      </c>
+      <c r="B131">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="C131" t="s">
+        <v>263</v>
+      </c>
+      <c r="D131" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <f t="shared" ref="A132:A191" si="4">A131+1</f>
+        <v>130</v>
+      </c>
+      <c r="B132">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="C132" t="s">
+        <v>264</v>
+      </c>
+      <c r="D132" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <f t="shared" si="4"/>
+        <v>131</v>
+      </c>
+      <c r="B133">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="C133" t="s">
+        <v>265</v>
+      </c>
+      <c r="D133" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <f t="shared" si="4"/>
+        <v>132</v>
+      </c>
+      <c r="B134">
+        <f t="shared" ref="B134:B184" si="5">FLOOR(A134/2,1)</f>
+        <v>66</v>
+      </c>
+      <c r="C134" t="s">
+        <v>266</v>
+      </c>
+      <c r="D134" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <f t="shared" si="4"/>
+        <v>133</v>
+      </c>
+      <c r="B135">
+        <f t="shared" si="5"/>
+        <v>66</v>
+      </c>
+      <c r="C135" t="s">
+        <v>267</v>
+      </c>
+      <c r="D135" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <f t="shared" si="4"/>
+        <v>134</v>
+      </c>
+      <c r="B136">
+        <f t="shared" si="5"/>
+        <v>67</v>
+      </c>
+      <c r="C136" t="s">
+        <v>268</v>
+      </c>
+      <c r="D136" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <f t="shared" si="4"/>
+        <v>135</v>
+      </c>
+      <c r="B137">
+        <f t="shared" si="5"/>
+        <v>67</v>
+      </c>
+      <c r="C137" t="s">
+        <v>269</v>
+      </c>
+      <c r="D137" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <f t="shared" si="4"/>
+        <v>136</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="5"/>
+        <v>68</v>
+      </c>
+      <c r="C138" t="s">
+        <v>270</v>
+      </c>
+      <c r="D138" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <f t="shared" si="4"/>
+        <v>137</v>
+      </c>
+      <c r="B139">
+        <f t="shared" si="5"/>
+        <v>68</v>
+      </c>
+      <c r="C139" t="s">
+        <v>271</v>
+      </c>
+      <c r="D139" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <f t="shared" si="4"/>
+        <v>138</v>
+      </c>
+      <c r="B140">
+        <f t="shared" si="5"/>
+        <v>69</v>
+      </c>
+      <c r="C140" t="s">
+        <v>272</v>
+      </c>
+      <c r="D140" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <f t="shared" si="4"/>
+        <v>139</v>
+      </c>
+      <c r="B141">
+        <f t="shared" si="5"/>
+        <v>69</v>
+      </c>
+      <c r="C141" t="s">
+        <v>273</v>
+      </c>
+      <c r="D141" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <f t="shared" si="4"/>
+        <v>140</v>
+      </c>
+      <c r="B142">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="C142" t="s">
+        <v>274</v>
+      </c>
+      <c r="D142" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <f t="shared" si="4"/>
+        <v>141</v>
+      </c>
+      <c r="B143">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="C143" t="s">
+        <v>275</v>
+      </c>
+      <c r="D143" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <f t="shared" si="4"/>
+        <v>142</v>
+      </c>
+      <c r="B144">
+        <f t="shared" si="5"/>
+        <v>71</v>
+      </c>
+      <c r="C144" t="s">
+        <v>276</v>
+      </c>
+      <c r="D144" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <f t="shared" si="4"/>
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <f t="shared" si="5"/>
+        <v>71</v>
+      </c>
+      <c r="C145" t="s">
+        <v>277</v>
+      </c>
+      <c r="D145" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
+      <c r="B146">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="C146" t="s">
+        <v>283</v>
+      </c>
+      <c r="D146" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <f t="shared" si="4"/>
+        <v>145</v>
+      </c>
+      <c r="B147">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="C147" t="s">
+        <v>284</v>
+      </c>
+      <c r="D147" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <f t="shared" si="4"/>
+        <v>146</v>
+      </c>
+      <c r="B148">
+        <f t="shared" si="5"/>
+        <v>73</v>
+      </c>
+      <c r="C148" t="s">
+        <v>285</v>
+      </c>
+      <c r="D148" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <f t="shared" si="4"/>
+        <v>147</v>
+      </c>
+      <c r="B149">
+        <f t="shared" si="5"/>
+        <v>73</v>
+      </c>
+      <c r="C149" t="s">
+        <v>286</v>
+      </c>
+      <c r="D149" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <f t="shared" si="4"/>
+        <v>148</v>
+      </c>
+      <c r="B150">
+        <f t="shared" si="5"/>
+        <v>74</v>
+      </c>
+      <c r="C150" t="s">
+        <v>244</v>
+      </c>
+      <c r="D150" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <f t="shared" si="4"/>
+        <v>149</v>
+      </c>
+      <c r="B151">
+        <f t="shared" si="5"/>
+        <v>74</v>
+      </c>
+      <c r="C151" t="s">
+        <v>245</v>
+      </c>
+      <c r="D151" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="B152">
+        <f t="shared" si="5"/>
+        <v>75</v>
+      </c>
+      <c r="C152" t="s">
+        <v>246</v>
+      </c>
+      <c r="D152" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <f t="shared" si="4"/>
+        <v>151</v>
+      </c>
+      <c r="B153">
+        <f t="shared" si="5"/>
+        <v>75</v>
+      </c>
+      <c r="C153" t="s">
+        <v>247</v>
+      </c>
+      <c r="D153" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <f t="shared" si="4"/>
+        <v>152</v>
+      </c>
+      <c r="B154">
+        <f t="shared" si="5"/>
+        <v>76</v>
+      </c>
+      <c r="C154" t="s">
+        <v>248</v>
+      </c>
+      <c r="D154" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <f t="shared" si="4"/>
+        <v>153</v>
+      </c>
+      <c r="B155">
+        <f t="shared" si="5"/>
+        <v>76</v>
+      </c>
+      <c r="C155" t="s">
+        <v>249</v>
+      </c>
+      <c r="D155" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <f t="shared" si="4"/>
+        <v>154</v>
+      </c>
+      <c r="B156">
+        <f t="shared" si="5"/>
+        <v>77</v>
+      </c>
+      <c r="C156" t="s">
+        <v>250</v>
+      </c>
+      <c r="D156" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <f t="shared" si="4"/>
+        <v>155</v>
+      </c>
+      <c r="B157">
+        <f t="shared" si="5"/>
+        <v>77</v>
+      </c>
+      <c r="C157" t="s">
+        <v>251</v>
+      </c>
+      <c r="D157" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <f t="shared" si="4"/>
+        <v>156</v>
+      </c>
+      <c r="B158">
+        <f t="shared" si="5"/>
+        <v>78</v>
+      </c>
+      <c r="C158" t="s">
+        <v>252</v>
+      </c>
+      <c r="D158" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <f t="shared" si="4"/>
+        <v>157</v>
+      </c>
+      <c r="B159">
+        <f t="shared" si="5"/>
+        <v>78</v>
+      </c>
+      <c r="C159" t="s">
+        <v>253</v>
+      </c>
+      <c r="D159" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <f t="shared" si="4"/>
+        <v>158</v>
+      </c>
+      <c r="B160">
+        <f t="shared" si="5"/>
+        <v>79</v>
+      </c>
+      <c r="C160" t="s">
+        <v>254</v>
+      </c>
+      <c r="D160" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <f t="shared" si="4"/>
+        <v>159</v>
+      </c>
+      <c r="B161">
+        <f t="shared" si="5"/>
+        <v>79</v>
+      </c>
+      <c r="C161" t="s">
+        <v>255</v>
+      </c>
+      <c r="D161" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="B162">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="C162" t="s">
+        <v>256</v>
+      </c>
+      <c r="D162" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <f t="shared" si="4"/>
+        <v>161</v>
+      </c>
+      <c r="B163">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="C163" t="s">
+        <v>257</v>
+      </c>
+      <c r="D163" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <f t="shared" si="4"/>
+        <v>162</v>
+      </c>
+      <c r="B164">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+      <c r="C164" t="s">
+        <v>258</v>
+      </c>
+      <c r="D164" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <f t="shared" si="4"/>
+        <v>163</v>
+      </c>
+      <c r="B165">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+      <c r="C165" t="s">
+        <v>259</v>
+      </c>
+      <c r="D165" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <f t="shared" si="4"/>
+        <v>164</v>
+      </c>
+      <c r="B166">
+        <f t="shared" si="5"/>
+        <v>82</v>
+      </c>
+      <c r="C166" t="s">
+        <v>260</v>
+      </c>
+      <c r="D166" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <f t="shared" si="4"/>
+        <v>165</v>
+      </c>
+      <c r="B167">
+        <f t="shared" si="5"/>
+        <v>82</v>
+      </c>
+      <c r="C167" t="s">
+        <v>279</v>
+      </c>
+      <c r="D167" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <f t="shared" si="4"/>
+        <v>166</v>
+      </c>
+      <c r="B168">
+        <f t="shared" si="5"/>
+        <v>83</v>
+      </c>
+      <c r="C168" t="s">
+        <v>280</v>
+      </c>
+      <c r="D168" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <f t="shared" si="4"/>
+        <v>167</v>
+      </c>
+      <c r="B169">
+        <f t="shared" si="5"/>
+        <v>83</v>
+      </c>
+      <c r="C169" t="s">
+        <v>281</v>
+      </c>
+      <c r="D169" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <f t="shared" si="4"/>
+        <v>168</v>
+      </c>
+      <c r="B170">
+        <f t="shared" si="5"/>
+        <v>84</v>
+      </c>
+      <c r="C170" t="s">
+        <v>282</v>
+      </c>
+      <c r="D170" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <f t="shared" si="4"/>
+        <v>169</v>
+      </c>
+      <c r="B171">
+        <f t="shared" si="5"/>
+        <v>84</v>
+      </c>
+      <c r="C171" t="s">
+        <v>261</v>
+      </c>
+      <c r="D171" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <f t="shared" si="4"/>
+        <v>170</v>
+      </c>
+      <c r="B172">
+        <f t="shared" si="5"/>
+        <v>85</v>
+      </c>
+      <c r="C172" t="s">
+        <v>262</v>
+      </c>
+      <c r="D172" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <f t="shared" si="4"/>
+        <v>171</v>
+      </c>
+      <c r="B173">
+        <f t="shared" si="5"/>
+        <v>85</v>
+      </c>
+      <c r="C173" t="s">
+        <v>263</v>
+      </c>
+      <c r="D173" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <f t="shared" si="4"/>
+        <v>172</v>
+      </c>
+      <c r="B174">
+        <f t="shared" si="5"/>
+        <v>86</v>
+      </c>
+      <c r="C174" t="s">
+        <v>264</v>
+      </c>
+      <c r="D174" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <f t="shared" si="4"/>
+        <v>173</v>
+      </c>
+      <c r="B175">
+        <f t="shared" si="5"/>
+        <v>86</v>
+      </c>
+      <c r="C175" t="s">
+        <v>265</v>
+      </c>
+      <c r="D175" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <f t="shared" si="4"/>
+        <v>174</v>
+      </c>
+      <c r="B176">
+        <f t="shared" si="5"/>
+        <v>87</v>
+      </c>
+      <c r="C176" t="s">
+        <v>266</v>
+      </c>
+      <c r="D176" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <f t="shared" si="4"/>
+        <v>175</v>
+      </c>
+      <c r="B177">
+        <f t="shared" si="5"/>
+        <v>87</v>
+      </c>
+      <c r="C177" t="s">
+        <v>267</v>
+      </c>
+      <c r="D177" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <f t="shared" si="4"/>
+        <v>176</v>
+      </c>
+      <c r="B178">
+        <f t="shared" si="5"/>
+        <v>88</v>
+      </c>
+      <c r="C178" t="s">
+        <v>268</v>
+      </c>
+      <c r="D178" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <f t="shared" si="4"/>
+        <v>177</v>
+      </c>
+      <c r="B179">
+        <f t="shared" si="5"/>
+        <v>88</v>
+      </c>
+      <c r="C179" t="s">
+        <v>269</v>
+      </c>
+      <c r="D179" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <f t="shared" si="4"/>
+        <v>178</v>
+      </c>
+      <c r="B180">
+        <f t="shared" si="5"/>
+        <v>89</v>
+      </c>
+      <c r="C180" t="s">
+        <v>270</v>
+      </c>
+      <c r="D180" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <f t="shared" si="4"/>
+        <v>179</v>
+      </c>
+      <c r="B181">
+        <f t="shared" si="5"/>
+        <v>89</v>
+      </c>
+      <c r="C181" t="s">
+        <v>271</v>
+      </c>
+      <c r="D181" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="B182">
+        <f t="shared" si="5"/>
+        <v>90</v>
+      </c>
+      <c r="C182" t="s">
+        <v>272</v>
+      </c>
+      <c r="D182" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <f t="shared" si="4"/>
+        <v>181</v>
+      </c>
+      <c r="B183">
+        <f t="shared" si="5"/>
+        <v>90</v>
+      </c>
+      <c r="C183" t="s">
+        <v>273</v>
+      </c>
+      <c r="D183" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <f t="shared" si="4"/>
+        <v>182</v>
+      </c>
+      <c r="B184">
+        <f t="shared" si="5"/>
+        <v>91</v>
+      </c>
+      <c r="C184" t="s">
+        <v>274</v>
+      </c>
+      <c r="D184" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <f t="shared" si="4"/>
+        <v>183</v>
+      </c>
+      <c r="B185">
+        <f t="shared" ref="B185:B191" si="6">FLOOR(A185/2,1)</f>
+        <v>91</v>
+      </c>
+      <c r="C185" t="s">
+        <v>275</v>
+      </c>
+      <c r="D185" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <f t="shared" si="4"/>
+        <v>184</v>
+      </c>
+      <c r="B186">
+        <f t="shared" si="6"/>
+        <v>92</v>
+      </c>
+      <c r="C186" t="s">
+        <v>276</v>
+      </c>
+      <c r="D186" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <f t="shared" si="4"/>
+        <v>185</v>
+      </c>
+      <c r="B187">
+        <f t="shared" si="6"/>
+        <v>92</v>
+      </c>
+      <c r="C187" t="s">
+        <v>277</v>
+      </c>
+      <c r="D187" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <f t="shared" si="4"/>
+        <v>186</v>
+      </c>
+      <c r="B188">
+        <f t="shared" si="6"/>
+        <v>93</v>
+      </c>
+      <c r="C188" t="s">
+        <v>283</v>
+      </c>
+      <c r="D188" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <f t="shared" si="4"/>
+        <v>187</v>
+      </c>
+      <c r="B189">
+        <f t="shared" si="6"/>
+        <v>93</v>
+      </c>
+      <c r="C189" t="s">
+        <v>284</v>
+      </c>
+      <c r="D189" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <f t="shared" si="4"/>
+        <v>188</v>
+      </c>
+      <c r="B190">
+        <f t="shared" si="6"/>
+        <v>94</v>
+      </c>
+      <c r="C190" t="s">
+        <v>285</v>
+      </c>
+      <c r="D190" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <f t="shared" si="4"/>
+        <v>189</v>
+      </c>
+      <c r="B191">
+        <f t="shared" si="6"/>
+        <v>94</v>
+      </c>
+      <c r="C191" t="s">
+        <v>286</v>
+      </c>
+      <c r="D191" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>